<commit_message>
Commit Caso de uso UC002 E UC005
</commit_message>
<xml_diff>
--- a/Requisitos/Template_Projeto.xlsx
+++ b/Requisitos/Template_Projeto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" codeName="EstaPasta_de_trabalho" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="601" activeTab="1"/>
+    <workbookView xWindow="1215" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="601" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="109">
   <si>
     <t>CAMPO</t>
   </si>
@@ -65,9 +65,6 @@
     <t>DADOS DE SAÍDA</t>
   </si>
   <si>
-    <t>CT002</t>
-  </si>
-  <si>
     <t>Projeto de Teste</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
   </si>
   <si>
     <t>Eduardo da hora lira</t>
-  </si>
-  <si>
-    <t>Berguisson ferreira</t>
   </si>
   <si>
     <t>SIB</t>
@@ -301,6 +295,87 @@
   </si>
   <si>
     <t>Senha foi alterada, digite novamente seus dados ou peça uma nova senha!</t>
+  </si>
+  <si>
+    <t>Usuario deve esta logado no sistema e o sistema esta conectado no Mercado de ações.</t>
+  </si>
+  <si>
+    <t>Atualizar cotações com sucesso.</t>
+  </si>
+  <si>
+    <t>dispare uma interrupção, a cada 5 minutos, indicando que as cotações devem ser atualizadas.</t>
+  </si>
+  <si>
+    <t>O sistema consulta as cotações das ações através da operadora do Mercado de Ações e atualiza o valor das ações, mantendo todo histórico dos valores das ações.</t>
+  </si>
+  <si>
+    <t>Testar requisito UC005 - Atualizar Cotações</t>
+  </si>
+  <si>
+    <t>Atualizar cotações SEM sucesso- DEVIDO AO TIMEOUT</t>
+  </si>
+  <si>
+    <t>Usuario deve esta logado no sistema e o sistema esta logado no Mercado de ações.</t>
+  </si>
+  <si>
+    <t>Atualizar cotações com sucesso- CANCELA OPERAÇÃO.</t>
+  </si>
+  <si>
+    <t>Cancele operação durante o disparo do relogio.</t>
+  </si>
+  <si>
+    <t>Em qualquer momento o usuário pode cancelar a operação. O caso de uso será encerrado.</t>
+  </si>
+  <si>
+    <t>Atualizar cotações com sucesso- DURANTE A CONSULTA CANCELE OPERAÇÃO.</t>
+  </si>
+  <si>
+    <t>Durante a consulta das cotações das ações será cancelado.</t>
+  </si>
+  <si>
+    <t>Em qualquer momento o usuário pode cancelar a operação. ocorrerá um timeout e o caso de uso será encerrado.</t>
+  </si>
+  <si>
+    <t>Atualizar cotações com sucesso- CANCELA OPERAÇÃO DURANTE O DISPARO DO RELOGIO.</t>
+  </si>
+  <si>
+    <t>Berguison ferreira</t>
+  </si>
+  <si>
+    <t>UC001</t>
+  </si>
+  <si>
+    <t>UC003</t>
+  </si>
+  <si>
+    <t>UC002</t>
+  </si>
+  <si>
+    <t>UC004</t>
+  </si>
+  <si>
+    <t>UC005</t>
+  </si>
+  <si>
+    <t>UC006</t>
+  </si>
+  <si>
+    <t>UC007</t>
+  </si>
+  <si>
+    <t>UC008</t>
+  </si>
+  <si>
+    <t>UC009</t>
+  </si>
+  <si>
+    <t>UC0010</t>
+  </si>
+  <si>
+    <t>UC0011</t>
+  </si>
+  <si>
+    <t>UC0012</t>
   </si>
 </sst>
 </file>
@@ -8589,7 +8664,7 @@
       <c r="C13" s="19"/>
       <c r="D13" s="28"/>
       <c r="E13" s="60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="60"/>
       <c r="G13" s="60"/>
@@ -8624,7 +8699,7 @@
       <c r="C16" s="19"/>
       <c r="D16" s="28"/>
       <c r="E16" s="61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="61"/>
       <c r="G16" s="61"/>
@@ -8649,7 +8724,7 @@
       <c r="D18" s="28"/>
       <c r="E18" s="33"/>
       <c r="F18" s="34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="33"/>
       <c r="H18" s="29"/>
@@ -8673,7 +8748,7 @@
       <c r="D20" s="28"/>
       <c r="E20" s="33"/>
       <c r="F20" s="35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" s="33"/>
       <c r="H20" s="29"/>
@@ -8686,7 +8761,7 @@
       <c r="D21" s="28"/>
       <c r="E21" s="33"/>
       <c r="F21" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="29"/>
@@ -8699,7 +8774,7 @@
       <c r="D22" s="28"/>
       <c r="E22" s="33"/>
       <c r="F22" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" s="33"/>
       <c r="H22" s="29"/>
@@ -8712,7 +8787,7 @@
       <c r="D23" s="28"/>
       <c r="E23" s="33"/>
       <c r="F23" s="35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" s="33"/>
       <c r="H23" s="29"/>
@@ -8725,7 +8800,7 @@
       <c r="D24" s="28"/>
       <c r="E24" s="33"/>
       <c r="F24" s="35" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="G24" s="33"/>
       <c r="H24" s="29"/>
@@ -8874,11 +8949,11 @@
   <sheetPr codeName="Plan3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:IH54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="M52" sqref="M52"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75"/>
@@ -8908,7 +8983,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="80" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="81"/>
       <c r="D1" s="82"/>
@@ -9162,28 +9237,28 @@
         <v>2</v>
       </c>
       <c r="B2" s="83" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="84"/>
       <c r="D2" s="85"/>
       <c r="E2" s="78"/>
       <c r="F2" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="92" t="s">
+      <c r="I2" s="92" t="s">
         <v>24</v>
-      </c>
-      <c r="H2" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="92" t="s">
-        <v>26</v>
       </c>
       <c r="J2" s="67"/>
       <c r="K2" s="67"/>
       <c r="L2" s="74"/>
       <c r="M2" s="71" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N2" s="64"/>
       <c r="O2" s="64"/>
@@ -9420,7 +9495,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="86" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="87"/>
       <c r="D3" s="88"/>
@@ -10406,20 +10481,20 @@
       <c r="IH6" s="1"/>
     </row>
     <row r="7" spans="1:242" s="9" customFormat="1" ht="33.75">
-      <c r="A7" s="62">
-        <v>1</v>
+      <c r="A7" s="62" t="s">
+        <v>97</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="99" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="99" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
@@ -10660,10 +10735,10 @@
       <c r="B8" s="63"/>
       <c r="C8" s="63"/>
       <c r="D8" s="100" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="100" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F8" s="96">
         <v>18333</v>
@@ -10672,16 +10747,16 @@
         <v>131313</v>
       </c>
       <c r="H8" s="98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
       <c r="L8" s="51"/>
       <c r="M8" s="52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N8" s="52"/>
       <c r="O8" s="52"/>
@@ -11403,19 +11478,19 @@
     </row>
     <row r="11" spans="1:242" s="9" customFormat="1" ht="51">
       <c r="A11" s="62" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E11" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
@@ -11660,28 +11735,28 @@
       <c r="B12" s="63"/>
       <c r="C12" s="63"/>
       <c r="D12" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="93" t="s">
         <v>36</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="93" t="s">
-        <v>38</v>
       </c>
       <c r="G12" s="93">
         <v>131313</v>
       </c>
       <c r="H12" s="94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I12" s="95" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J12" s="50"/>
       <c r="K12" s="50"/>
       <c r="L12" s="51"/>
       <c r="M12" s="52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N12" s="53"/>
       <c r="O12" s="53"/>
@@ -12402,20 +12477,20 @@
       <c r="IH14"/>
     </row>
     <row r="15" spans="1:242" s="9" customFormat="1" ht="51">
-      <c r="A15" s="62">
-        <v>3</v>
+      <c r="A15" s="62" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F15" s="49"/>
       <c r="G15" s="50"/>
@@ -12660,28 +12735,28 @@
       <c r="B16" s="63"/>
       <c r="C16" s="63"/>
       <c r="D16" s="48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F16" s="101">
         <v>18333</v>
       </c>
       <c r="G16" s="101" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H16" s="94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I16" s="95" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J16" s="50"/>
       <c r="K16" s="50"/>
       <c r="L16" s="51"/>
       <c r="M16" s="52" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N16" s="53"/>
       <c r="O16" s="53"/>
@@ -13402,20 +13477,20 @@
       <c r="IH18"/>
     </row>
     <row r="19" spans="1:242" s="9" customFormat="1" ht="51">
-      <c r="A19" s="62">
-        <v>4</v>
+      <c r="A19" s="62" t="s">
+        <v>100</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E19" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="49"/>
       <c r="G19" s="50"/>
@@ -13660,10 +13735,10 @@
       <c r="B20" s="63"/>
       <c r="C20" s="63"/>
       <c r="D20" s="48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E20" s="48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20" s="102">
         <v>18333</v>
@@ -13672,16 +13747,16 @@
         <v>131313</v>
       </c>
       <c r="H20" s="94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I20" s="95" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J20" s="50"/>
       <c r="K20" s="50"/>
       <c r="L20" s="51"/>
       <c r="M20" s="52" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N20" s="53"/>
       <c r="O20" s="53"/>
@@ -14402,20 +14477,20 @@
       <c r="IH22"/>
     </row>
     <row r="23" spans="1:242" ht="12.75" customHeight="1">
-      <c r="A23" s="62">
-        <v>5</v>
+      <c r="A23" s="62" t="s">
+        <v>101</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E23" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F23" s="49"/>
       <c r="G23" s="50"/>
@@ -14435,10 +14510,10 @@
       <c r="B24" s="63"/>
       <c r="C24" s="63"/>
       <c r="D24" s="48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F24" s="102">
         <v>18333</v>
@@ -14447,16 +14522,16 @@
         <v>131313</v>
       </c>
       <c r="H24" s="94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I24" s="95" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J24" s="50"/>
       <c r="K24" s="50"/>
       <c r="L24" s="51"/>
       <c r="M24" s="52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N24" s="53"/>
       <c r="O24" s="53"/>
@@ -14502,20 +14577,20 @@
       <c r="Q26" s="58"/>
     </row>
     <row r="27" spans="1:242" ht="51">
-      <c r="A27" s="62">
-        <v>6</v>
+      <c r="A27" s="62" t="s">
+        <v>102</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E27" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F27" s="49"/>
       <c r="G27" s="50"/>
@@ -14535,28 +14610,28 @@
       <c r="B28" s="63"/>
       <c r="C28" s="63"/>
       <c r="D28" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="102" t="s">
-        <v>50</v>
-      </c>
       <c r="G28" s="103" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H28" s="103" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I28" s="103" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J28" s="50"/>
       <c r="K28" s="50"/>
       <c r="L28" s="51"/>
       <c r="M28" s="52" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N28" s="53"/>
       <c r="O28" s="53"/>
@@ -14602,20 +14677,20 @@
       <c r="Q30" s="58"/>
     </row>
     <row r="31" spans="1:242" ht="12.75" customHeight="1">
-      <c r="A31" s="62">
-        <v>7</v>
+      <c r="A31" s="62" t="s">
+        <v>103</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D31" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E31" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F31" s="49"/>
       <c r="G31" s="50"/>
@@ -14635,10 +14710,10 @@
       <c r="B32" s="63"/>
       <c r="C32" s="63"/>
       <c r="D32" s="48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E32" s="48" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F32" s="93">
         <v>18333</v>
@@ -14647,16 +14722,16 @@
         <v>131313</v>
       </c>
       <c r="H32" s="94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I32" s="95" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J32" s="50"/>
       <c r="K32" s="50"/>
       <c r="L32" s="51"/>
       <c r="M32" s="52" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N32" s="53"/>
       <c r="O32" s="53"/>
@@ -14702,20 +14777,20 @@
       <c r="Q34" s="58"/>
     </row>
     <row r="35" spans="1:17" ht="51">
-      <c r="A35" s="62">
-        <v>8</v>
+      <c r="A35" s="62" t="s">
+        <v>104</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D35" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E35" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F35" s="49"/>
       <c r="G35" s="50"/>
@@ -14735,10 +14810,10 @@
       <c r="B36" s="63"/>
       <c r="C36" s="63"/>
       <c r="D36" s="48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E36" s="48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F36" s="93">
         <v>18333</v>
@@ -14747,16 +14822,16 @@
         <v>131313</v>
       </c>
       <c r="H36" s="93" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I36" s="95" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J36" s="50"/>
       <c r="K36" s="50"/>
       <c r="L36" s="51"/>
       <c r="M36" s="52" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N36" s="53"/>
       <c r="O36" s="53"/>
@@ -14802,20 +14877,20 @@
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17" ht="51">
-      <c r="A39" s="62">
-        <v>9</v>
+      <c r="A39" s="62" t="s">
+        <v>105</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D39" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E39" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F39" s="49"/>
       <c r="G39" s="50"/>
@@ -14835,10 +14910,10 @@
       <c r="B40" s="63"/>
       <c r="C40" s="63"/>
       <c r="D40" s="48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E40" s="48" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F40" s="93">
         <v>18333</v>
@@ -14847,16 +14922,16 @@
         <v>131313</v>
       </c>
       <c r="H40" s="94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I40" s="95" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J40" s="50"/>
       <c r="K40" s="50"/>
       <c r="L40" s="51"/>
       <c r="M40" s="52" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N40" s="53"/>
       <c r="O40" s="53"/>
@@ -14902,20 +14977,20 @@
       <c r="Q42" s="58"/>
     </row>
     <row r="43" spans="1:17" ht="51">
-      <c r="A43" s="62">
-        <v>10</v>
+      <c r="A43" s="62" t="s">
+        <v>106</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C43" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E43" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F43" s="49"/>
       <c r="G43" s="50"/>
@@ -14935,10 +15010,10 @@
       <c r="B44" s="63"/>
       <c r="C44" s="63"/>
       <c r="D44" s="48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E44" s="48" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F44" s="93">
         <v>18333</v>
@@ -14947,16 +15022,16 @@
         <v>131313</v>
       </c>
       <c r="H44" s="94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I44" s="95" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J44" s="50"/>
       <c r="K44" s="50"/>
       <c r="L44" s="51"/>
       <c r="M44" s="52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N44" s="53"/>
       <c r="O44" s="53"/>
@@ -15002,20 +15077,20 @@
       <c r="Q46" s="58"/>
     </row>
     <row r="47" spans="1:17" ht="51">
-      <c r="A47" s="62">
-        <v>11</v>
+      <c r="A47" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="B47" s="63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C47" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E47" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F47" s="49"/>
       <c r="G47" s="50"/>
@@ -15035,10 +15110,10 @@
       <c r="B48" s="63"/>
       <c r="C48" s="63"/>
       <c r="D48" s="48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E48" s="48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F48" s="93">
         <v>18333</v>
@@ -15047,16 +15122,16 @@
         <v>131313</v>
       </c>
       <c r="H48" s="94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I48" s="95" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J48" s="50"/>
       <c r="K48" s="50"/>
       <c r="L48" s="51"/>
       <c r="M48" s="52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N48" s="53"/>
       <c r="O48" s="53"/>
@@ -15102,20 +15177,20 @@
       <c r="Q50" s="58"/>
     </row>
     <row r="51" spans="1:17" ht="51">
-      <c r="A51" s="62">
-        <v>12</v>
+      <c r="A51" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="B51" s="63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C51" s="63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E51" s="48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F51" s="49"/>
       <c r="G51" s="50"/>
@@ -15135,10 +15210,10 @@
       <c r="B52" s="63"/>
       <c r="C52" s="63"/>
       <c r="D52" s="48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E52" s="48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F52" s="49"/>
       <c r="G52" s="49"/>
@@ -15148,7 +15223,7 @@
       <c r="K52" s="50"/>
       <c r="L52" s="51"/>
       <c r="M52" s="52" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N52" s="53"/>
       <c r="O52" s="53"/>
@@ -16173,7 +16248,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q54"/>
+      <selection activeCell="A7" sqref="A7:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -16315,8 +16390,8 @@
       <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="62">
-        <v>1</v>
+      <c r="A7" s="62" t="s">
+        <v>97</v>
       </c>
       <c r="B7" s="63"/>
       <c r="C7" s="63"/>
@@ -16394,7 +16469,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="62" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -16471,8 +16546,8 @@
       <c r="Q14" s="58"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="62">
-        <v>3</v>
+      <c r="A15" s="62" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -16549,8 +16624,8 @@
       <c r="Q18" s="58"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="62">
-        <v>4</v>
+      <c r="A19" s="62" t="s">
+        <v>100</v>
       </c>
       <c r="B19" s="63"/>
       <c r="C19" s="63"/>
@@ -16627,8 +16702,8 @@
       <c r="Q22" s="58"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="62">
-        <v>5</v>
+      <c r="A23" s="62" t="s">
+        <v>101</v>
       </c>
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
@@ -16705,8 +16780,8 @@
       <c r="Q26" s="58"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="62">
-        <v>6</v>
+      <c r="A27" s="62" t="s">
+        <v>102</v>
       </c>
       <c r="B27" s="63"/>
       <c r="C27" s="63"/>
@@ -16783,8 +16858,8 @@
       <c r="Q30" s="58"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="62">
-        <v>7</v>
+      <c r="A31" s="62" t="s">
+        <v>103</v>
       </c>
       <c r="B31" s="63"/>
       <c r="C31" s="63"/>
@@ -16861,8 +16936,8 @@
       <c r="Q34" s="58"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="62">
-        <v>8</v>
+      <c r="A35" s="62" t="s">
+        <v>104</v>
       </c>
       <c r="B35" s="63"/>
       <c r="C35" s="63"/>
@@ -16939,8 +17014,8 @@
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="62">
-        <v>9</v>
+      <c r="A39" s="62" t="s">
+        <v>105</v>
       </c>
       <c r="B39" s="63"/>
       <c r="C39" s="63"/>
@@ -17017,8 +17092,8 @@
       <c r="Q42" s="58"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="62">
-        <v>10</v>
+      <c r="A43" s="62" t="s">
+        <v>106</v>
       </c>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -17095,8 +17170,8 @@
       <c r="Q46" s="58"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="62">
-        <v>11</v>
+      <c r="A47" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="B47" s="63"/>
       <c r="C47" s="63"/>
@@ -17173,8 +17248,8 @@
       <c r="Q50" s="58"/>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="62">
-        <v>12</v>
+      <c r="A51" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="B51" s="63"/>
       <c r="C51" s="63"/>
@@ -18196,7 +18271,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q54"/>
+      <selection activeCell="A7" sqref="A7:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -18338,8 +18413,8 @@
       <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="62">
-        <v>1</v>
+      <c r="A7" s="62" t="s">
+        <v>97</v>
       </c>
       <c r="B7" s="63"/>
       <c r="C7" s="63"/>
@@ -18417,7 +18492,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="62" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -18494,8 +18569,8 @@
       <c r="Q14" s="58"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="62">
-        <v>3</v>
+      <c r="A15" s="62" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -18572,8 +18647,8 @@
       <c r="Q18" s="58"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="62">
-        <v>4</v>
+      <c r="A19" s="62" t="s">
+        <v>100</v>
       </c>
       <c r="B19" s="63"/>
       <c r="C19" s="63"/>
@@ -18650,8 +18725,8 @@
       <c r="Q22" s="58"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="62">
-        <v>5</v>
+      <c r="A23" s="62" t="s">
+        <v>101</v>
       </c>
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
@@ -18728,8 +18803,8 @@
       <c r="Q26" s="58"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="62">
-        <v>6</v>
+      <c r="A27" s="62" t="s">
+        <v>102</v>
       </c>
       <c r="B27" s="63"/>
       <c r="C27" s="63"/>
@@ -18806,8 +18881,8 @@
       <c r="Q30" s="58"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="62">
-        <v>7</v>
+      <c r="A31" s="62" t="s">
+        <v>103</v>
       </c>
       <c r="B31" s="63"/>
       <c r="C31" s="63"/>
@@ -18884,8 +18959,8 @@
       <c r="Q34" s="58"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="62">
-        <v>8</v>
+      <c r="A35" s="62" t="s">
+        <v>104</v>
       </c>
       <c r="B35" s="63"/>
       <c r="C35" s="63"/>
@@ -18962,8 +19037,8 @@
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="62">
-        <v>9</v>
+      <c r="A39" s="62" t="s">
+        <v>105</v>
       </c>
       <c r="B39" s="63"/>
       <c r="C39" s="63"/>
@@ -19040,8 +19115,8 @@
       <c r="Q42" s="58"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="62">
-        <v>10</v>
+      <c r="A43" s="62" t="s">
+        <v>106</v>
       </c>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -19118,8 +19193,8 @@
       <c r="Q46" s="58"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="62">
-        <v>11</v>
+      <c r="A47" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="B47" s="63"/>
       <c r="C47" s="63"/>
@@ -19196,8 +19271,8 @@
       <c r="Q50" s="58"/>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="62">
-        <v>12</v>
+      <c r="A51" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="B51" s="63"/>
       <c r="C51" s="63"/>
@@ -20218,8 +20293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:Q54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -20361,8 +20436,8 @@
       <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="62">
-        <v>1</v>
+      <c r="A7" s="62" t="s">
+        <v>97</v>
       </c>
       <c r="B7" s="63"/>
       <c r="C7" s="63"/>
@@ -20440,7 +20515,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="62" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -20517,8 +20592,8 @@
       <c r="Q14" s="58"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="62">
-        <v>3</v>
+      <c r="A15" s="62" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -20595,8 +20670,8 @@
       <c r="Q18" s="58"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="62">
-        <v>4</v>
+      <c r="A19" s="62" t="s">
+        <v>100</v>
       </c>
       <c r="B19" s="63"/>
       <c r="C19" s="63"/>
@@ -20673,8 +20748,8 @@
       <c r="Q22" s="58"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="62">
-        <v>5</v>
+      <c r="A23" s="62" t="s">
+        <v>101</v>
       </c>
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
@@ -20751,8 +20826,8 @@
       <c r="Q26" s="58"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="62">
-        <v>6</v>
+      <c r="A27" s="62" t="s">
+        <v>102</v>
       </c>
       <c r="B27" s="63"/>
       <c r="C27" s="63"/>
@@ -20829,8 +20904,8 @@
       <c r="Q30" s="58"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="62">
-        <v>7</v>
+      <c r="A31" s="62" t="s">
+        <v>103</v>
       </c>
       <c r="B31" s="63"/>
       <c r="C31" s="63"/>
@@ -20907,8 +20982,8 @@
       <c r="Q34" s="58"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="62">
-        <v>8</v>
+      <c r="A35" s="62" t="s">
+        <v>104</v>
       </c>
       <c r="B35" s="63"/>
       <c r="C35" s="63"/>
@@ -20985,8 +21060,8 @@
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="62">
-        <v>9</v>
+      <c r="A39" s="62" t="s">
+        <v>105</v>
       </c>
       <c r="B39" s="63"/>
       <c r="C39" s="63"/>
@@ -21063,8 +21138,8 @@
       <c r="Q42" s="58"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="62">
-        <v>10</v>
+      <c r="A43" s="62" t="s">
+        <v>106</v>
       </c>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -21141,8 +21216,8 @@
       <c r="Q46" s="58"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="62">
-        <v>11</v>
+      <c r="A47" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="B47" s="63"/>
       <c r="C47" s="63"/>
@@ -21219,8 +21294,8 @@
       <c r="Q50" s="58"/>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="62">
-        <v>12</v>
+      <c r="A51" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="B51" s="63"/>
       <c r="C51" s="63"/>
@@ -22241,11 +22316,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q54"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="59" t="s">
@@ -22299,7 +22380,9 @@
       <c r="A3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="86"/>
+      <c r="B3" s="86" t="s">
+        <v>86</v>
+      </c>
       <c r="C3" s="87"/>
       <c r="D3" s="88"/>
       <c r="E3" s="78"/>
@@ -22383,14 +22466,22 @@
       <c r="P6" s="47"/>
       <c r="Q6" s="42"/>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="62">
-        <v>1</v>
-      </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+    <row r="7" spans="1:17" ht="89.25" customHeight="1">
+      <c r="A7" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>85</v>
+      </c>
       <c r="F7" s="49"/>
       <c r="G7" s="50"/>
       <c r="H7" s="50"/>
@@ -22461,14 +22552,22 @@
       <c r="P10" s="57"/>
       <c r="Q10" s="58"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" ht="92.25" customHeight="1">
       <c r="A11" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+        <v>99</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>85</v>
+      </c>
       <c r="F11" s="49"/>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
@@ -22539,14 +22638,22 @@
       <c r="P14" s="57"/>
       <c r="Q14" s="58"/>
     </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="62">
-        <v>3</v>
-      </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
+    <row r="15" spans="1:17" ht="55.5" customHeight="1">
+      <c r="A15" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>91</v>
+      </c>
       <c r="F15" s="49"/>
       <c r="G15" s="50"/>
       <c r="H15" s="50"/>
@@ -22617,14 +22724,22 @@
       <c r="P18" s="57"/>
       <c r="Q18" s="58"/>
     </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="62">
-        <v>4</v>
-      </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
+    <row r="19" spans="1:17" ht="63.75" customHeight="1">
+      <c r="A19" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>94</v>
+      </c>
       <c r="F19" s="49"/>
       <c r="G19" s="50"/>
       <c r="H19" s="50"/>
@@ -22695,14 +22810,22 @@
       <c r="P22" s="57"/>
       <c r="Q22" s="58"/>
     </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="62">
-        <v>5</v>
-      </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
+    <row r="23" spans="1:17" ht="51" customHeight="1">
+      <c r="A23" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="48" t="s">
+        <v>90</v>
+      </c>
       <c r="F23" s="49"/>
       <c r="G23" s="50"/>
       <c r="H23" s="50"/>
@@ -22774,8 +22897,8 @@
       <c r="Q26" s="58"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="62">
-        <v>6</v>
+      <c r="A27" s="62" t="s">
+        <v>102</v>
       </c>
       <c r="B27" s="63"/>
       <c r="C27" s="63"/>
@@ -22852,8 +22975,8 @@
       <c r="Q30" s="58"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="62">
-        <v>7</v>
+      <c r="A31" s="62" t="s">
+        <v>103</v>
       </c>
       <c r="B31" s="63"/>
       <c r="C31" s="63"/>
@@ -22930,8 +23053,8 @@
       <c r="Q34" s="58"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="62">
-        <v>8</v>
+      <c r="A35" s="62" t="s">
+        <v>104</v>
       </c>
       <c r="B35" s="63"/>
       <c r="C35" s="63"/>
@@ -23008,8 +23131,8 @@
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="62">
-        <v>9</v>
+      <c r="A39" s="62" t="s">
+        <v>105</v>
       </c>
       <c r="B39" s="63"/>
       <c r="C39" s="63"/>
@@ -23086,8 +23209,8 @@
       <c r="Q42" s="58"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="62">
-        <v>10</v>
+      <c r="A43" s="62" t="s">
+        <v>106</v>
       </c>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -23164,8 +23287,8 @@
       <c r="Q46" s="58"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="62">
-        <v>11</v>
+      <c r="A47" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="B47" s="63"/>
       <c r="C47" s="63"/>
@@ -23242,8 +23365,8 @@
       <c r="Q50" s="58"/>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="62">
-        <v>12</v>
+      <c r="A51" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="B51" s="63"/>
       <c r="C51" s="63"/>
@@ -24265,7 +24388,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q54"/>
+      <selection activeCell="A7" sqref="A7:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -24407,8 +24530,8 @@
       <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="62">
-        <v>1</v>
+      <c r="A7" s="62" t="s">
+        <v>97</v>
       </c>
       <c r="B7" s="63"/>
       <c r="C7" s="63"/>
@@ -24486,7 +24609,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="62" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -24563,8 +24686,8 @@
       <c r="Q14" s="58"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="62">
-        <v>3</v>
+      <c r="A15" s="62" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -24641,8 +24764,8 @@
       <c r="Q18" s="58"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="62">
-        <v>4</v>
+      <c r="A19" s="62" t="s">
+        <v>100</v>
       </c>
       <c r="B19" s="63"/>
       <c r="C19" s="63"/>
@@ -24719,8 +24842,8 @@
       <c r="Q22" s="58"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="62">
-        <v>5</v>
+      <c r="A23" s="62" t="s">
+        <v>101</v>
       </c>
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
@@ -24797,8 +24920,8 @@
       <c r="Q26" s="58"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="62">
-        <v>6</v>
+      <c r="A27" s="62" t="s">
+        <v>102</v>
       </c>
       <c r="B27" s="63"/>
       <c r="C27" s="63"/>
@@ -24875,8 +24998,8 @@
       <c r="Q30" s="58"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="62">
-        <v>7</v>
+      <c r="A31" s="62" t="s">
+        <v>103</v>
       </c>
       <c r="B31" s="63"/>
       <c r="C31" s="63"/>
@@ -24953,8 +25076,8 @@
       <c r="Q34" s="58"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="62">
-        <v>8</v>
+      <c r="A35" s="62" t="s">
+        <v>104</v>
       </c>
       <c r="B35" s="63"/>
       <c r="C35" s="63"/>
@@ -25031,8 +25154,8 @@
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="62">
-        <v>9</v>
+      <c r="A39" s="62" t="s">
+        <v>105</v>
       </c>
       <c r="B39" s="63"/>
       <c r="C39" s="63"/>
@@ -25109,8 +25232,8 @@
       <c r="Q42" s="58"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="62">
-        <v>10</v>
+      <c r="A43" s="62" t="s">
+        <v>106</v>
       </c>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -25187,8 +25310,8 @@
       <c r="Q46" s="58"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="62">
-        <v>11</v>
+      <c r="A47" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="B47" s="63"/>
       <c r="C47" s="63"/>
@@ -25265,8 +25388,8 @@
       <c r="Q50" s="58"/>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="62">
-        <v>12</v>
+      <c r="A51" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="B51" s="63"/>
       <c r="C51" s="63"/>
@@ -26287,8 +26410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -26430,8 +26553,8 @@
       <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="62">
-        <v>1</v>
+      <c r="A7" s="62" t="s">
+        <v>97</v>
       </c>
       <c r="B7" s="63"/>
       <c r="C7" s="63"/>
@@ -26509,7 +26632,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="62" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -26586,8 +26709,8 @@
       <c r="Q14" s="58"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="62">
-        <v>3</v>
+      <c r="A15" s="62" t="s">
+        <v>98</v>
       </c>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -26664,8 +26787,8 @@
       <c r="Q18" s="58"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="62">
-        <v>4</v>
+      <c r="A19" s="62" t="s">
+        <v>100</v>
       </c>
       <c r="B19" s="63"/>
       <c r="C19" s="63"/>
@@ -26742,8 +26865,8 @@
       <c r="Q22" s="58"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="62">
-        <v>5</v>
+      <c r="A23" s="62" t="s">
+        <v>101</v>
       </c>
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
@@ -26820,8 +26943,8 @@
       <c r="Q26" s="58"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="62">
-        <v>6</v>
+      <c r="A27" s="62" t="s">
+        <v>102</v>
       </c>
       <c r="B27" s="63"/>
       <c r="C27" s="63"/>
@@ -26898,8 +27021,8 @@
       <c r="Q30" s="58"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="62">
-        <v>7</v>
+      <c r="A31" s="62" t="s">
+        <v>103</v>
       </c>
       <c r="B31" s="63"/>
       <c r="C31" s="63"/>
@@ -26976,8 +27099,8 @@
       <c r="Q34" s="58"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="62">
-        <v>8</v>
+      <c r="A35" s="62" t="s">
+        <v>104</v>
       </c>
       <c r="B35" s="63"/>
       <c r="C35" s="63"/>
@@ -27054,8 +27177,8 @@
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="62">
-        <v>9</v>
+      <c r="A39" s="62" t="s">
+        <v>105</v>
       </c>
       <c r="B39" s="63"/>
       <c r="C39" s="63"/>
@@ -27132,8 +27255,8 @@
       <c r="Q42" s="58"/>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="62">
-        <v>10</v>
+      <c r="A43" s="62" t="s">
+        <v>106</v>
       </c>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -27210,8 +27333,8 @@
       <c r="Q46" s="58"/>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="62">
-        <v>11</v>
+      <c r="A47" s="62" t="s">
+        <v>107</v>
       </c>
       <c r="B47" s="63"/>
       <c r="C47" s="63"/>
@@ -27288,8 +27411,8 @@
       <c r="Q50" s="58"/>
     </row>
     <row r="51" spans="1:17">
-      <c r="A51" s="62">
-        <v>12</v>
+      <c r="A51" s="62" t="s">
+        <v>108</v>
       </c>
       <c r="B51" s="63"/>
       <c r="C51" s="63"/>

</xml_diff>

<commit_message>
padronizando cenarios versao 2
</commit_message>
<xml_diff>
--- a/Requisitos/Template_Projeto.xlsx
+++ b/Requisitos/Template_Projeto.xlsx
@@ -39898,11 +39898,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:A53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="12.75" customHeight="1">
       <c r="A1" s="87" t="s">
@@ -40067,7 +40073,7 @@
       <c r="E7" s="136" t="s">
         <v>239</v>
       </c>
-      <c r="F7" s="137" t="s">
+      <c r="F7" s="150" t="s">
         <v>240</v>
       </c>
       <c r="G7" s="138"/>
@@ -40162,7 +40168,7 @@
       <c r="F11" s="137" t="s">
         <v>244</v>
       </c>
-      <c r="G11" s="137" t="s">
+      <c r="G11" s="150" t="s">
         <v>245</v>
       </c>
       <c r="H11" s="137" t="s">
@@ -40439,7 +40445,7 @@
         <f>F11</f>
         <v>Agencia</v>
       </c>
-      <c r="G23" s="137" t="str">
+      <c r="G23" s="150" t="str">
         <f>G11</f>
         <v>Numero Conta</v>
       </c>
@@ -40910,10 +40916,10 @@
       <c r="F43" s="150" t="s">
         <v>276</v>
       </c>
-      <c r="G43" s="137" t="s">
+      <c r="G43" s="150" t="s">
         <v>277</v>
       </c>
-      <c r="H43" s="137" t="s">
+      <c r="H43" s="150" t="s">
         <v>278</v>
       </c>
       <c r="I43" s="138"/>
@@ -41003,10 +41009,10 @@
       <c r="F47" s="150" t="s">
         <v>282</v>
       </c>
-      <c r="G47" s="137" t="s">
+      <c r="G47" s="150" t="s">
         <v>277</v>
       </c>
-      <c r="H47" s="137" t="s">
+      <c r="H47" s="150" t="s">
         <v>278</v>
       </c>
       <c r="I47" s="138"/>
@@ -41097,7 +41103,7 @@
       <c r="F51" s="150" t="s">
         <v>284</v>
       </c>
-      <c r="G51" s="137" t="s">
+      <c r="G51" s="150" t="s">
         <v>285</v>
       </c>
       <c r="H51" s="138"/>

</xml_diff>

<commit_message>
correcoes ortograficas no UC007
</commit_message>
<xml_diff>
--- a/Requisitos/Template_Projeto.xlsx
+++ b/Requisitos/Template_Projeto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="601" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="1215" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="601" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="289">
   <si>
     <t>CAMPO</t>
   </si>
@@ -1226,9 +1226,6 @@
     <t>Saldo Conta</t>
   </si>
   <si>
-    <t>Testar requisito UC006 - comprar acões</t>
-  </si>
-  <si>
     <t>Comprar ações com saldo insuficiente</t>
   </si>
   <si>
@@ -1278,9 +1275,6 @@
       </rPr>
       <t xml:space="preserve"> (BOVESPA, NASDAQ, MERVAL )</t>
     </r>
-  </si>
-  <si>
-    <t>para cada tipo de ação o sistema deve aprensentar quantidade de ações disponivel para compra</t>
   </si>
   <si>
     <t>BOVESPA</t>
@@ -2022,13 +2016,7 @@
     <t>O sistema informará conforme dados de saída.</t>
   </si>
   <si>
-    <t>Cliqui com Mouse</t>
-  </si>
-  <si>
     <t>Tela realizar DOC</t>
-  </si>
-  <si>
-    <t>Validar dados usuario logado</t>
   </si>
   <si>
     <t>Sistema informará Conforme dados de entrada.</t>
@@ -2052,13 +2040,7 @@
     <t>O sistema canelará o DOC</t>
   </si>
   <si>
-    <t>Cliqui no Botão [Cancelar DOC]</t>
-  </si>
-  <si>
     <t>Validar dados para realizar DOC</t>
-  </si>
-  <si>
-    <t>Informar  o número da agência, o número da conta, tipo do DOC, valor DOC, data de tranferência, nome favorecido, cpf ou cgc, senha.</t>
   </si>
   <si>
     <t>Não haver erro de validação.</t>
@@ -2094,12 +2076,6 @@
     <t>Validar data incorreta</t>
   </si>
   <si>
-    <t>Data de tranferência, no formato desconhecido</t>
-  </si>
-  <si>
-    <t>Data de tranferência, anterior a atual</t>
-  </si>
-  <si>
     <t>"Data incorreta, digite novamente a senha."</t>
   </si>
   <si>
@@ -2113,18 +2089,6 @@
   </si>
   <si>
     <t>Confirmar Transferência</t>
-  </si>
-  <si>
-    <t>O sistema realizará a tranferência</t>
-  </si>
-  <si>
-    <t>Cliqui no Botão [Confirmar]</t>
-  </si>
-  <si>
-    <t>Validar dados do comprovante do usuário rea lizou transferência</t>
-  </si>
-  <si>
-    <t>Sistema informará dados do usuário que está realizando a tranferência conforme dados de entrada.</t>
   </si>
   <si>
     <t>Dados informado pelo sistema igual as dados do usuário logado.</t>
@@ -2142,16 +2106,10 @@
     <t>Validar dados do comprovante do cliente recebeu transferência</t>
   </si>
   <si>
-    <t>Sistema informará dados do cliente que recebeu a tranferência conforme dados de entrada.</t>
-  </si>
-  <si>
     <t>Dados informado pelo sistema igual as dados informados pelo  usuário .</t>
   </si>
   <si>
     <t>Nome Cliente</t>
-  </si>
-  <si>
-    <t>Validar valor e data tranferência</t>
   </si>
   <si>
     <t>Data transferência</t>
@@ -2164,6 +2122,51 @@
   </si>
   <si>
     <t>CT0012</t>
+  </si>
+  <si>
+    <t>Clique com Mouse</t>
+  </si>
+  <si>
+    <t>Validar dados usuário logado</t>
+  </si>
+  <si>
+    <t>Clique no Botão [Cancelar DOC]</t>
+  </si>
+  <si>
+    <t>Informar  o número da agência, o número da conta, tipo do DOC, valor DOC, data de transferência, nome favorecido, cpf ou cgc, senha.</t>
+  </si>
+  <si>
+    <t>Data de transferência, no formato desconhecido</t>
+  </si>
+  <si>
+    <t>Data de transferência, anterior a atual</t>
+  </si>
+  <si>
+    <t>O sistema realizará a transferência</t>
+  </si>
+  <si>
+    <t>Clique no Botão [Confirmar]</t>
+  </si>
+  <si>
+    <t>Sistema informará dados do usuário que está realizando a transferência conforme dados de entrada.</t>
+  </si>
+  <si>
+    <t>Sistema informará dados do cliente que recebeu a transferência conforme dados de entrada.</t>
+  </si>
+  <si>
+    <t>Validar valor e data transferência</t>
+  </si>
+  <si>
+    <t>Validar dados do comprovante do usuário realizou transferência</t>
+  </si>
+  <si>
+    <t>Testar requisito UC006 - comprar ações</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esta logado no sistema, (ter efetuado Login e esta cadastrado para comprar ações )   </t>
+  </si>
+  <si>
+    <t>para cada tipo de ação o sistema deve apresentar quantidade de ações disponível para compra</t>
   </si>
 </sst>
 </file>
@@ -11715,7 +11718,7 @@
     </row>
     <row r="7" spans="1:242" s="9" customFormat="1" ht="63.75">
       <c r="A7" s="91" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B7" s="92" t="s">
         <v>50</v>
@@ -13715,7 +13718,7 @@
     </row>
     <row r="15" spans="1:242" s="9" customFormat="1" ht="63.75">
       <c r="A15" s="91" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B15" s="92" t="s">
         <v>78</v>
@@ -14715,7 +14718,7 @@
     </row>
     <row r="19" spans="1:242" s="9" customFormat="1" ht="63.75">
       <c r="A19" s="90" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B19" s="92" t="s">
         <v>75</v>
@@ -15715,7 +15718,7 @@
     </row>
     <row r="23" spans="1:242" ht="60" customHeight="1">
       <c r="A23" s="90" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" s="92" t="s">
         <v>73</v>
@@ -15815,7 +15818,7 @@
     </row>
     <row r="27" spans="1:242" ht="63.75">
       <c r="A27" s="90" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B27" s="92" t="s">
         <v>67</v>
@@ -15915,7 +15918,7 @@
     </row>
     <row r="31" spans="1:242" ht="60.75" customHeight="1">
       <c r="A31" s="90" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B31" s="92" t="s">
         <v>65</v>
@@ -16015,7 +16018,7 @@
     </row>
     <row r="35" spans="1:17" ht="63.75">
       <c r="A35" s="90" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B35" s="92" t="s">
         <v>59</v>
@@ -16115,10 +16118,10 @@
     </row>
     <row r="39" spans="1:17" ht="63.75">
       <c r="A39" s="90" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B39" s="92" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C39" s="93" t="s">
         <v>28</v>
@@ -16147,10 +16150,10 @@
       <c r="B40" s="93"/>
       <c r="C40" s="93"/>
       <c r="D40" s="60" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E40" s="60" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F40" s="50">
         <v>18333</v>
@@ -16168,7 +16171,7 @@
       <c r="K40" s="50"/>
       <c r="L40" s="51"/>
       <c r="M40" s="52" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="N40" s="53"/>
       <c r="O40" s="53"/>
@@ -16215,7 +16218,7 @@
     </row>
     <row r="43" spans="1:17" ht="63.75">
       <c r="A43" s="90" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B43" s="92" t="s">
         <v>47</v>
@@ -16262,7 +16265,7 @@
         <v>25</v>
       </c>
       <c r="I44" s="50" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J44" s="50"/>
       <c r="K44" s="50"/>
@@ -16315,7 +16318,7 @@
     </row>
     <row r="47" spans="1:17" ht="63.75">
       <c r="A47" s="90" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B47" s="92" t="s">
         <v>46</v>
@@ -16347,7 +16350,7 @@
       <c r="B48" s="93"/>
       <c r="C48" s="93"/>
       <c r="D48" s="60" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E48" s="60" t="s">
         <v>51</v>
@@ -25390,10 +25393,10 @@
       <c r="D2" s="118"/>
       <c r="E2" s="111"/>
       <c r="F2" s="97" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G2" s="97" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H2" s="97"/>
       <c r="I2" s="97"/>
@@ -25404,7 +25407,7 @@
         <v>95</v>
       </c>
       <c r="N2" s="94" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="O2" s="94"/>
       <c r="P2" s="94"/>
@@ -25415,7 +25418,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="123" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C3" s="120"/>
       <c r="D3" s="121"/>
@@ -25502,19 +25505,19 @@
     </row>
     <row r="7" spans="1:17" ht="80.25" customHeight="1">
       <c r="A7" s="91" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B7" s="92" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="92" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="60" t="s">
         <v>205</v>
       </c>
-      <c r="C7" s="92" t="s">
+      <c r="E7" s="60" t="s">
         <v>206</v>
-      </c>
-      <c r="D7" s="60" t="s">
-        <v>207</v>
-      </c>
-      <c r="E7" s="60" t="s">
-        <v>208</v>
       </c>
       <c r="F7" s="71"/>
       <c r="G7" s="72"/>
@@ -25534,16 +25537,16 @@
       <c r="B8" s="93"/>
       <c r="C8" s="93"/>
       <c r="D8" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="F8" s="71" t="s">
         <v>209</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="G8" s="72" t="s">
         <v>210</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>211</v>
-      </c>
-      <c r="G8" s="72" t="s">
-        <v>212</v>
       </c>
       <c r="H8" s="50"/>
       <c r="I8" s="49"/>
@@ -25552,7 +25555,7 @@
       <c r="L8" s="51"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
@@ -25563,10 +25566,10 @@
       <c r="B9" s="93"/>
       <c r="C9" s="93"/>
       <c r="D9" s="60" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
@@ -25577,7 +25580,7 @@
       <c r="L9" s="51"/>
       <c r="M9" s="53"/>
       <c r="N9" s="52" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O9" s="53"/>
       <c r="P9" s="53"/>
@@ -25607,16 +25610,16 @@
         <v>114</v>
       </c>
       <c r="B11" s="92" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="92" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" s="60" t="s">
         <v>217</v>
-      </c>
-      <c r="C11" s="92" t="s">
-        <v>206</v>
-      </c>
-      <c r="D11" s="60" t="s">
-        <v>218</v>
-      </c>
-      <c r="E11" s="60" t="s">
-        <v>219</v>
       </c>
       <c r="F11" s="71"/>
       <c r="G11" s="71"/>
@@ -25636,13 +25639,13 @@
       <c r="B12" s="93"/>
       <c r="C12" s="93"/>
       <c r="D12" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" s="71" t="s">
         <v>209</v>
-      </c>
-      <c r="E12" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="F12" s="71" t="s">
-        <v>211</v>
       </c>
       <c r="G12" s="71" t="s">
         <v>32</v>
@@ -25653,7 +25656,7 @@
       <c r="K12" s="50"/>
       <c r="L12" s="51"/>
       <c r="M12" s="52" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N12" s="53"/>
       <c r="O12" s="53"/>
@@ -25700,19 +25703,19 @@
     </row>
     <row r="15" spans="1:17" ht="86.25" customHeight="1">
       <c r="A15" s="91" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C15" s="92" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="60" t="s">
         <v>206</v>
-      </c>
-      <c r="D15" s="60" t="s">
-        <v>218</v>
-      </c>
-      <c r="E15" s="60" t="s">
-        <v>208</v>
       </c>
       <c r="F15" s="71"/>
       <c r="G15" s="71"/>
@@ -25732,16 +25735,16 @@
       <c r="B16" s="93"/>
       <c r="C16" s="93"/>
       <c r="D16" s="60" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E16" s="60" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F16" s="71" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G16" s="71" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H16" s="50"/>
       <c r="I16" s="50"/>
@@ -25749,7 +25752,7 @@
       <c r="K16" s="50"/>
       <c r="L16" s="51"/>
       <c r="M16" s="52" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N16" s="53"/>
       <c r="O16" s="53"/>
@@ -25796,25 +25799,25 @@
     </row>
     <row r="19" spans="1:17" ht="111.75" customHeight="1">
       <c r="A19" s="91" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C19" s="92" t="s">
+        <v>204</v>
+      </c>
+      <c r="D19" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="60" t="s">
         <v>206</v>
       </c>
-      <c r="D19" s="60" t="s">
-        <v>218</v>
-      </c>
-      <c r="E19" s="60" t="s">
-        <v>208</v>
-      </c>
       <c r="F19" s="71" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G19" s="71" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H19" s="50"/>
       <c r="I19" s="50"/>
@@ -25832,10 +25835,10 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="60" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E20" s="60" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F20" s="49"/>
       <c r="G20" s="49"/>
@@ -25845,10 +25848,10 @@
       <c r="K20" s="50"/>
       <c r="L20" s="51"/>
       <c r="M20" s="52" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N20" s="52" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="O20" s="53"/>
       <c r="P20" s="53"/>
@@ -28088,7 +28091,7 @@
       <c r="D2" s="118"/>
       <c r="E2" s="111"/>
       <c r="F2" s="97" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G2" s="97"/>
       <c r="H2" s="97"/>
@@ -28097,10 +28100,10 @@
       <c r="K2" s="97"/>
       <c r="L2" s="106"/>
       <c r="M2" s="102" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N2" s="94" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="O2" s="94"/>
       <c r="P2" s="94"/>
@@ -28111,7 +28114,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="127" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3" s="120"/>
       <c r="D3" s="121"/>
@@ -28198,22 +28201,22 @@
     </row>
     <row r="7" spans="1:17" ht="78.75" customHeight="1">
       <c r="A7" s="124" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B7" s="92" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="125" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="E7" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="F7" s="71" t="s">
         <v>192</v>
-      </c>
-      <c r="E7" s="60" t="s">
-        <v>193</v>
-      </c>
-      <c r="F7" s="71" t="s">
-        <v>194</v>
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="50"/>
@@ -28232,10 +28235,10 @@
       <c r="B8" s="93"/>
       <c r="C8" s="93"/>
       <c r="D8" s="60" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F8" s="49"/>
       <c r="G8" s="49"/>
@@ -28245,10 +28248,10 @@
       <c r="K8" s="50"/>
       <c r="L8" s="51"/>
       <c r="M8" s="52" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N8" s="52" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
@@ -28297,19 +28300,19 @@
         <v>114</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C11" s="125" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="60" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="60" t="s">
-        <v>200</v>
-      </c>
-      <c r="E11" s="60" t="s">
-        <v>193</v>
-      </c>
       <c r="F11" s="71" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
@@ -28328,10 +28331,10 @@
       <c r="B12" s="93"/>
       <c r="C12" s="93"/>
       <c r="D12" s="60" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F12" s="49"/>
       <c r="G12" s="49"/>
@@ -28341,10 +28344,10 @@
       <c r="K12" s="50"/>
       <c r="L12" s="51"/>
       <c r="M12" s="52" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N12" s="52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O12" s="53"/>
       <c r="P12" s="53"/>
@@ -30277,13 +30280,13 @@
     </row>
     <row r="7" spans="1:17" ht="89.25" customHeight="1">
       <c r="A7" s="91" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B7" s="93" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="93" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D7" s="48" t="s">
         <v>37</v>
@@ -30368,19 +30371,19 @@
         <v>114</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="93" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D11" s="48" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F11" s="71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
@@ -30389,7 +30392,7 @@
       <c r="K11" s="50"/>
       <c r="L11" s="51"/>
       <c r="M11" s="52" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="N11" s="52"/>
       <c r="O11" s="52"/>
@@ -30455,22 +30458,22 @@
     </row>
     <row r="15" spans="1:17" ht="66" customHeight="1">
       <c r="A15" s="91" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C15" s="93" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E15" s="60" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F15" s="71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G15" s="50"/>
       <c r="H15" s="50"/>
@@ -30545,22 +30548,22 @@
     </row>
     <row r="19" spans="1:17" ht="91.5" customHeight="1">
       <c r="A19" s="91" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C19" s="93" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D19" s="60" t="s">
         <v>40</v>
       </c>
       <c r="E19" s="60" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F19" s="71" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G19" s="50"/>
       <c r="H19" s="50"/>
@@ -30569,7 +30572,7 @@
       <c r="K19" s="50"/>
       <c r="L19" s="51"/>
       <c r="M19" s="52" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N19" s="52"/>
       <c r="O19" s="52"/>
@@ -30635,22 +30638,22 @@
     </row>
     <row r="23" spans="1:17" ht="51" customHeight="1">
       <c r="A23" s="91" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" s="92" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="93" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="60" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="60" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="71" t="s">
         <v>161</v>
-      </c>
-      <c r="C23" s="93" t="s">
-        <v>175</v>
-      </c>
-      <c r="D23" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="E23" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="F23" s="71" t="s">
-        <v>163</v>
       </c>
       <c r="G23" s="50"/>
       <c r="H23" s="50"/>
@@ -31104,11 +31107,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:II33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75"/>
@@ -31656,7 +31659,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="123" t="s">
-        <v>135</v>
+        <v>286</v>
       </c>
       <c r="C3" s="120"/>
       <c r="D3" s="121"/>
@@ -32650,16 +32653,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="92" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" s="93" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="E7" s="73" t="s">
         <v>138</v>
-      </c>
-      <c r="E7" s="73" t="s">
-        <v>139</v>
       </c>
       <c r="F7" s="71"/>
       <c r="G7" s="72"/>
@@ -32672,7 +32675,7 @@
       <c r="N7" s="52"/>
       <c r="O7" s="52"/>
       <c r="P7" s="52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q7" s="52"/>
       <c r="R7" s="38"/>
@@ -32907,13 +32910,13 @@
       <c r="B8" s="92"/>
       <c r="C8" s="93"/>
       <c r="D8" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>288</v>
+      </c>
+      <c r="F8" s="71" t="s">
         <v>141</v>
-      </c>
-      <c r="E8" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>143</v>
       </c>
       <c r="G8" s="72"/>
       <c r="H8" s="72"/>
@@ -32923,7 +32926,7 @@
       <c r="L8" s="51"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
@@ -33161,7 +33164,7 @@
       <c r="C9" s="93"/>
       <c r="D9" s="60"/>
       <c r="E9" s="75" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="72"/>
@@ -33408,7 +33411,7 @@
       <c r="C10" s="93"/>
       <c r="D10" s="60"/>
       <c r="E10" s="60" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F10" s="71"/>
       <c r="G10" s="72"/>
@@ -33422,7 +33425,7 @@
       <c r="O10" s="52"/>
       <c r="P10" s="52"/>
       <c r="Q10" s="52" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="R10" s="38"/>
       <c r="S10" s="13"/>
@@ -33657,7 +33660,7 @@
       <c r="C11" s="93"/>
       <c r="D11" s="60"/>
       <c r="E11" s="75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
@@ -33667,7 +33670,7 @@
       <c r="K11" s="50"/>
       <c r="L11" s="51"/>
       <c r="M11" s="52" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="N11" s="52"/>
       <c r="O11" s="52"/>
@@ -34150,16 +34153,16 @@
         <v>114</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C13" s="93" t="s">
+        <v>287</v>
+      </c>
+      <c r="D13" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="E13" s="73" t="s">
         <v>138</v>
-      </c>
-      <c r="E13" s="73" t="s">
-        <v>139</v>
       </c>
       <c r="F13" s="71"/>
       <c r="G13" s="72"/>
@@ -34172,7 +34175,7 @@
       <c r="N13" s="52"/>
       <c r="O13" s="52"/>
       <c r="P13" s="52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q13" s="52"/>
       <c r="R13" s="38"/>
@@ -34407,13 +34410,13 @@
       <c r="B14" s="92"/>
       <c r="C14" s="93"/>
       <c r="D14" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="74" t="s">
+        <v>288</v>
+      </c>
+      <c r="F14" s="71" t="s">
         <v>141</v>
-      </c>
-      <c r="E14" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" s="71" t="s">
-        <v>143</v>
       </c>
       <c r="G14" s="72"/>
       <c r="H14" s="72"/>
@@ -34423,7 +34426,7 @@
       <c r="L14" s="51"/>
       <c r="M14" s="52"/>
       <c r="N14" s="52" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O14" s="52"/>
       <c r="P14" s="52"/>
@@ -34661,7 +34664,7 @@
       <c r="C15" s="93"/>
       <c r="D15" s="60"/>
       <c r="E15" s="75" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F15" s="71"/>
       <c r="G15" s="72"/>
@@ -34908,7 +34911,7 @@
       <c r="C16" s="93"/>
       <c r="D16" s="60"/>
       <c r="E16" s="60" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F16" s="71"/>
       <c r="G16" s="72"/>
@@ -34922,7 +34925,7 @@
       <c r="O16" s="53"/>
       <c r="P16" s="53"/>
       <c r="Q16" s="52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="R16" s="38"/>
       <c r="S16" s="13"/>
@@ -35157,7 +35160,7 @@
       <c r="C17" s="93"/>
       <c r="D17" s="60"/>
       <c r="E17" s="60" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F17" s="50"/>
       <c r="G17" s="50"/>
@@ -35167,7 +35170,7 @@
       <c r="K17" s="50"/>
       <c r="L17" s="51"/>
       <c r="M17" s="52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N17" s="53"/>
       <c r="O17" s="53"/>
@@ -35650,16 +35653,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="93" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C19" s="93" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="E19" s="73" t="s">
         <v>138</v>
-      </c>
-      <c r="E19" s="73" t="s">
-        <v>139</v>
       </c>
       <c r="F19" s="71"/>
       <c r="G19" s="50"/>
@@ -35672,7 +35675,7 @@
       <c r="N19" s="52"/>
       <c r="O19" s="52"/>
       <c r="P19" s="52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q19" s="52"/>
       <c r="R19" s="38"/>
@@ -35907,13 +35910,13 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="74" t="s">
+        <v>288</v>
+      </c>
+      <c r="F20" s="71" t="s">
         <v>141</v>
-      </c>
-      <c r="E20" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20" s="71" t="s">
-        <v>143</v>
       </c>
       <c r="G20" s="72"/>
       <c r="H20" s="50"/>
@@ -35923,7 +35926,7 @@
       <c r="L20" s="51"/>
       <c r="M20" s="52"/>
       <c r="N20" s="52" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O20" s="52"/>
       <c r="P20" s="52"/>
@@ -36161,7 +36164,7 @@
       <c r="C21" s="93"/>
       <c r="D21" s="48"/>
       <c r="E21" s="75" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F21" s="49"/>
       <c r="G21" s="49"/>
@@ -36408,7 +36411,7 @@
       <c r="C22" s="93"/>
       <c r="D22" s="48"/>
       <c r="E22" s="60" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F22" s="49"/>
       <c r="G22" s="49"/>
@@ -36422,7 +36425,7 @@
       <c r="O22" s="53"/>
       <c r="P22" s="53"/>
       <c r="Q22" s="52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="R22" s="38"/>
       <c r="S22" s="13"/>
@@ -36657,7 +36660,7 @@
       <c r="C23" s="93"/>
       <c r="D23" s="48"/>
       <c r="E23" s="60" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F23" s="49"/>
       <c r="G23" s="49"/>
@@ -36904,7 +36907,7 @@
       <c r="C24" s="93"/>
       <c r="D24" s="48"/>
       <c r="E24" s="60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F24" s="49"/>
       <c r="G24" s="49"/>
@@ -37151,7 +37154,7 @@
       <c r="C25" s="93"/>
       <c r="D25" s="48"/>
       <c r="E25" s="60" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F25" s="49"/>
       <c r="G25" s="49"/>
@@ -37398,7 +37401,7 @@
       <c r="C26" s="93"/>
       <c r="D26" s="48"/>
       <c r="E26" s="60" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F26" s="50"/>
       <c r="G26" s="50"/>
@@ -37410,7 +37413,7 @@
       <c r="M26" s="52"/>
       <c r="N26" s="53"/>
       <c r="O26" s="52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P26" s="53"/>
       <c r="Q26" s="53"/>
@@ -39898,15 +39901,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -39964,10 +39974,10 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="87" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B3" s="131" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C3" s="114"/>
       <c r="D3" s="115"/>
@@ -39990,7 +40000,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="132" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C4" s="117"/>
       <c r="D4" s="118"/>
@@ -40056,25 +40066,25 @@
       <c r="P6" s="47"/>
       <c r="Q6" s="42"/>
     </row>
-    <row r="7" spans="1:17" ht="102">
+    <row r="7" spans="1:17" ht="63.75">
       <c r="A7" s="133" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B7" s="134" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C7" s="135" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D7" s="136" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E7" s="136" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F7" s="150" t="s">
-        <v>240</v>
+        <v>274</v>
       </c>
       <c r="G7" s="138"/>
       <c r="H7" s="138"/>
@@ -40083,7 +40093,7 @@
       <c r="K7" s="138"/>
       <c r="L7" s="51"/>
       <c r="M7" s="139" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="N7" s="139"/>
       <c r="O7" s="139"/>
@@ -40152,34 +40162,34 @@
         <v>114</v>
       </c>
       <c r="B11" s="134" t="s">
-        <v>242</v>
+        <v>275</v>
       </c>
       <c r="C11" s="135" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D11" s="136" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E11" s="136" t="str">
         <f>E7</f>
         <v>O sistema informará conforme dados de saída.</v>
       </c>
       <c r="F11" s="137" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G11" s="150" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H11" s="137" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I11" s="137"/>
       <c r="J11" s="138"/>
       <c r="K11" s="138"/>
       <c r="L11" s="51"/>
       <c r="M11" s="139" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="N11" s="139"/>
       <c r="O11" s="139"/>
@@ -40245,10 +40255,10 @@
     </row>
     <row r="15" spans="1:17" ht="63.75">
       <c r="A15" s="149" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B15" s="134" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C15" s="135"/>
       <c r="D15" s="141" t="str">
@@ -40256,10 +40266,10 @@
         <v>Sistema informará Conforme dados de entrada.</v>
       </c>
       <c r="E15" s="136" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F15" s="150" t="s">
-        <v>250</v>
+        <v>276</v>
       </c>
       <c r="G15" s="137"/>
       <c r="H15" s="137"/>
@@ -40335,20 +40345,20 @@
     </row>
     <row r="19" spans="1:17" ht="216.75">
       <c r="A19" s="149" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B19" s="134" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C19" s="140" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D19" s="136" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="E19" s="136" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="F19" s="137"/>
       <c r="G19" s="137"/>
@@ -40368,10 +40378,10 @@
       <c r="B20" s="140"/>
       <c r="C20" s="140"/>
       <c r="D20" s="136" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E20" s="136" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F20" s="150"/>
       <c r="G20" s="150"/>
@@ -40426,20 +40436,20 @@
     </row>
     <row r="23" spans="1:17" ht="102">
       <c r="A23" s="149" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" s="134" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C23" s="140" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D23" s="136" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E23" s="136" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F23" s="137" t="str">
         <f>F11</f>
@@ -40458,7 +40468,7 @@
       <c r="K23" s="138"/>
       <c r="L23" s="51"/>
       <c r="M23" s="139" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="N23" s="139"/>
       <c r="O23" s="139"/>
@@ -40524,10 +40534,10 @@
     </row>
     <row r="27" spans="1:17" ht="102">
       <c r="A27" s="149" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B27" s="134" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C27" s="140" t="str">
         <f>B3</f>
@@ -40542,7 +40552,7 @@
         <v>o sistema informará uma mensagem Conforme dados de saída.</v>
       </c>
       <c r="F27" s="150" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="G27" s="138"/>
       <c r="H27" s="138"/>
@@ -40551,7 +40561,7 @@
       <c r="K27" s="138"/>
       <c r="L27" s="51"/>
       <c r="M27" s="139" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="N27" s="139" t="str">
         <f>M11</f>
@@ -40620,10 +40630,10 @@
     </row>
     <row r="31" spans="1:17" ht="102">
       <c r="A31" s="149" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B31" s="134" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C31" s="140" t="str">
         <f>B3</f>
@@ -40638,10 +40648,10 @@
         <v>o sistema informará uma mensagem Conforme dados de saída.</v>
       </c>
       <c r="F31" s="150" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="G31" s="150" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="H31" s="150"/>
       <c r="I31" s="138"/>
@@ -40649,7 +40659,7 @@
       <c r="K31" s="138"/>
       <c r="L31" s="51"/>
       <c r="M31" s="139" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="N31" s="139"/>
       <c r="O31" s="139"/>
@@ -40715,10 +40725,10 @@
     </row>
     <row r="35" spans="1:17" ht="102">
       <c r="A35" s="149" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B35" s="134" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C35" s="140" t="str">
         <f>C31</f>
@@ -40733,7 +40743,7 @@
         <v>o sistema informará uma mensagem Conforme dados de saída.</v>
       </c>
       <c r="F35" s="150" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="G35" s="138"/>
       <c r="H35" s="138"/>
@@ -40742,7 +40752,7 @@
       <c r="K35" s="138"/>
       <c r="L35" s="51"/>
       <c r="M35" s="139" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="N35" s="139"/>
       <c r="O35" s="139"/>
@@ -40808,10 +40818,10 @@
     </row>
     <row r="39" spans="1:17" ht="76.5">
       <c r="A39" s="149" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B39" s="134" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C39" s="140" t="str">
         <f>C35</f>
@@ -40822,10 +40832,10 @@
         <v>Informar conforme dados de entrada.</v>
       </c>
       <c r="E39" s="136" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="F39" s="150" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="G39" s="138"/>
       <c r="H39" s="138"/>
@@ -40898,29 +40908,29 @@
     </row>
     <row r="43" spans="1:17" ht="153">
       <c r="A43" s="149" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="B43" s="134" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C43" s="140" t="str">
         <f>C39</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D43" s="136" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="E43" s="136" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="F43" s="150" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="G43" s="150" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="H43" s="150" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="I43" s="138"/>
       <c r="J43" s="138"/>
@@ -40991,29 +41001,29 @@
     </row>
     <row r="47" spans="1:17" ht="140.25">
       <c r="A47" s="149" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B47" s="134" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="C47" s="140" t="str">
         <f>C43</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D47" s="136" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E47" s="136" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="F47" s="150" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="G47" s="150" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="H47" s="150" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="I47" s="138"/>
       <c r="J47" s="138"/>
@@ -41084,10 +41094,10 @@
     </row>
     <row r="51" spans="1:17" ht="114.75">
       <c r="A51" s="149" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="B51" s="134" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C51" s="140" t="str">
         <f>C47</f>
@@ -41098,13 +41108,13 @@
         <v>Sistema informará Conforme dados de entrada.</v>
       </c>
       <c r="E51" s="136" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="F51" s="150" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="G51" s="150" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="H51" s="138"/>
       <c r="I51" s="138"/>

</xml_diff>

<commit_message>
padronizando UC003 e UC004
</commit_message>
<xml_diff>
--- a/Requisitos/Template_Projeto.xlsx
+++ b/Requisitos/Template_Projeto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="601" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="1215" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="601" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="5" r:id="rId1"/>
@@ -1649,67 +1649,7 @@
     <t>Ter logado no sistema e informado dados do cartão SIB card com sucesso conforme o UC003 - CT001</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">selecionar qual tipo da consulta opção </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;  Extrato de conta corrente</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">sistema libera a opção </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&gt; digitar a data para o extrato </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e libera o botão consultar.</t>
-    </r>
-  </si>
-  <si>
     <t>18/11/2013</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">clicar no botão </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[consultar]</t>
-    </r>
-  </si>
-  <si>
-    <t>visualização dos dados bancarios, nome e transações da data escolhida como nos dados de saida</t>
   </si>
   <si>
     <t xml:space="preserve">Nome: Jose Reis Agencia: 5565      CC: 10000       </t>
@@ -1729,20 +1669,6 @@
         <family val="2"/>
       </rPr>
       <t>&gt;Extrato de conta poupança</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">selecionar qual tipo da consulta opção </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;  Extrato de conta poupança</t>
     </r>
   </si>
   <si>
@@ -1778,45 +1704,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">o sistema disponibiliza as caixas para preenchimento das opções </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt; dados, numero de cartão e senha</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">preencher campos conforme os dados de entrada e clicar no botão </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>[consultar cartão]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>sistema informa conforme os dados de saida</t>
-  </si>
-  <si>
     <t>1234.5678.9023.4567</t>
   </si>
   <si>
@@ -1840,12 +1727,6 @@
     </r>
   </si>
   <si>
-    <t>sistema disponibiliza os histórico completo do cliente descrino na UC004 dependendo do tipo de consulta</t>
-  </si>
-  <si>
-    <t>histórico de dados e debitos do cartão dependendo do tipo de consulta conforme UC004</t>
-  </si>
-  <si>
     <t>Senha invalida</t>
   </si>
   <si>
@@ -1863,45 +1744,13 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">o sistema disponibiliza as caixas para preenchimento </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt; dados, numero de cartão e senha</t>
-    </r>
-  </si>
-  <si>
-    <t>sistema informa conforme os dados de saida e retorna para prenchimento dos dados novamente.</t>
-  </si>
-  <si>
-    <t>"senha inválida  digite novamente o cartão e senha"</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Numero do cartão inválido</t>
-  </si>
-  <si>
-    <t>sistema informa conforme os dados de saida e retorna para tela inicial do sistema.</t>
   </si>
   <si>
     <t>0000.0000.0000.0000</t>
   </si>
   <si>
-    <t>"cartão inexistente operação cancelada"</t>
-  </si>
-  <si>
     <t>Operadora fora de operação</t>
-  </si>
-  <si>
-    <t>"não foi possível se conectar a operadora tente novamente mais tarde"</t>
-  </si>
-  <si>
-    <t>inicio do sistema SIB</t>
   </si>
   <si>
     <r>
@@ -2167,6 +2016,157 @@
   </si>
   <si>
     <t>para cada tipo de ação o sistema deve apresentar quantidade de ações disponível para compra</t>
+  </si>
+  <si>
+    <t>Inicio do sistema SIB</t>
+  </si>
+  <si>
+    <t>Histórico de dados e debitos do cartão dependendo do tipo de consulta conforme UC004</t>
+  </si>
+  <si>
+    <t>"Senha inválida  digite novamente o cartão e senha"</t>
+  </si>
+  <si>
+    <t>"Cartão inexistente operação cancelada"</t>
+  </si>
+  <si>
+    <t>"Não foi possível se conectar a operadora tente novamente mais tarde"</t>
+  </si>
+  <si>
+    <t>O sistema informa conforme os dados de saida e retorna para tela inicial do sistema.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema disponibiliza as caixas para preenchimento das opções </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt; dados, numero de cartão e senha</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema informa conforme os dados de saida e retorna para prenchimento dos dados novamente.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema disponibiliza as caixas para preenchimento </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt; dados, numero de cartão e senha</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema disponibiliza os histórico completo do cliente descrino na UC004 dependendo do tipo de consulta</t>
+  </si>
+  <si>
+    <t>O sistema informa conforme os dados de saida</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Preencher campos conforme os dados de entrada e clicar no botão </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[consultar cartão]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Visualização dos dados bancarios, nome e transações da data escolhida como nos dados de saida</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O sistema libera a opção </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; digitar a data para o extrato </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e libera o botão consultar.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Selecionar qual tipo da consulta opção </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;  Extrato de conta corrente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clicar no botão </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>[consultar]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Selecionar qual tipo da consulta opção </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;  Extrato de conta poupança</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -10186,7 +10186,7 @@
   <dimension ref="A1:IH54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
       <selection pane="bottomRight" activeCell="B58" sqref="B58"/>
@@ -16121,7 +16121,7 @@
         <v>170</v>
       </c>
       <c r="B39" s="92" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="C39" s="93" t="s">
         <v>28</v>
@@ -16150,10 +16150,10 @@
       <c r="B40" s="93"/>
       <c r="C40" s="93"/>
       <c r="D40" s="60" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="E40" s="60" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="F40" s="50">
         <v>18333</v>
@@ -16171,7 +16171,7 @@
       <c r="K40" s="50"/>
       <c r="L40" s="51"/>
       <c r="M40" s="52" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="N40" s="53"/>
       <c r="O40" s="53"/>
@@ -16350,7 +16350,7 @@
       <c r="B48" s="93"/>
       <c r="C48" s="93"/>
       <c r="D48" s="60" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="E48" s="60" t="s">
         <v>51</v>
@@ -25376,8 +25376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -25436,10 +25436,10 @@
       <c r="D2" s="118"/>
       <c r="E2" s="111"/>
       <c r="F2" s="97" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G2" s="97" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H2" s="97"/>
       <c r="I2" s="97"/>
@@ -25461,7 +25461,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="123" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C3" s="120"/>
       <c r="D3" s="121"/>
@@ -25551,16 +25551,16 @@
         <v>163</v>
       </c>
       <c r="B7" s="92" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C7" s="92" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D7" s="60" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>206</v>
+        <v>278</v>
       </c>
       <c r="F7" s="71"/>
       <c r="G7" s="72"/>
@@ -25580,16 +25580,16 @@
       <c r="B8" s="93"/>
       <c r="C8" s="93"/>
       <c r="D8" s="60" t="s">
-        <v>207</v>
+        <v>283</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>208</v>
+        <v>282</v>
       </c>
       <c r="F8" s="71" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G8" s="72" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H8" s="50"/>
       <c r="I8" s="49"/>
@@ -25598,7 +25598,7 @@
       <c r="L8" s="51"/>
       <c r="M8" s="52"/>
       <c r="N8" s="52" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
@@ -25609,10 +25609,10 @@
       <c r="B9" s="93"/>
       <c r="C9" s="93"/>
       <c r="D9" s="60" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>213</v>
+        <v>281</v>
       </c>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
@@ -25623,7 +25623,7 @@
       <c r="L9" s="51"/>
       <c r="M9" s="53"/>
       <c r="N9" s="52" t="s">
-        <v>214</v>
+        <v>273</v>
       </c>
       <c r="O9" s="53"/>
       <c r="P9" s="53"/>
@@ -25653,16 +25653,16 @@
         <v>114</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C11" s="92" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D11" s="60" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>217</v>
+        <v>280</v>
       </c>
       <c r="F11" s="71"/>
       <c r="G11" s="71"/>
@@ -25682,13 +25682,13 @@
       <c r="B12" s="93"/>
       <c r="C12" s="93"/>
       <c r="D12" s="60" t="s">
-        <v>207</v>
+        <v>283</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>218</v>
+        <v>279</v>
       </c>
       <c r="F12" s="71" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G12" s="71" t="s">
         <v>32</v>
@@ -25699,7 +25699,7 @@
       <c r="K12" s="50"/>
       <c r="L12" s="51"/>
       <c r="M12" s="52" t="s">
-        <v>219</v>
+        <v>274</v>
       </c>
       <c r="N12" s="53"/>
       <c r="O12" s="53"/>
@@ -25749,16 +25749,16 @@
         <v>164</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="C15" s="92" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D15" s="60" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E15" s="60" t="s">
-        <v>206</v>
+        <v>278</v>
       </c>
       <c r="F15" s="71"/>
       <c r="G15" s="71"/>
@@ -25778,16 +25778,16 @@
       <c r="B16" s="93"/>
       <c r="C16" s="93"/>
       <c r="D16" s="60" t="s">
-        <v>207</v>
+        <v>283</v>
       </c>
       <c r="E16" s="60" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F16" s="71" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="G16" s="71" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H16" s="50"/>
       <c r="I16" s="50"/>
@@ -25795,7 +25795,7 @@
       <c r="K16" s="50"/>
       <c r="L16" s="51"/>
       <c r="M16" s="52" t="s">
-        <v>223</v>
+        <v>275</v>
       </c>
       <c r="N16" s="53"/>
       <c r="O16" s="53"/>
@@ -25845,22 +25845,22 @@
         <v>165</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C19" s="92" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D19" s="60" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E19" s="60" t="s">
-        <v>206</v>
+        <v>278</v>
       </c>
       <c r="F19" s="71" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G19" s="71" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H19" s="50"/>
       <c r="I19" s="50"/>
@@ -25878,10 +25878,10 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="60" t="s">
-        <v>207</v>
+        <v>283</v>
       </c>
       <c r="E20" s="60" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F20" s="49"/>
       <c r="G20" s="49"/>
@@ -25891,10 +25891,10 @@
       <c r="K20" s="50"/>
       <c r="L20" s="51"/>
       <c r="M20" s="52" t="s">
-        <v>225</v>
+        <v>276</v>
       </c>
       <c r="N20" s="52" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="O20" s="53"/>
       <c r="P20" s="53"/>
@@ -26806,8 +26806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -26984,13 +26984,13 @@
         <v>189</v>
       </c>
       <c r="D7" s="60" t="s">
+        <v>286</v>
+      </c>
+      <c r="E7" s="60" t="s">
+        <v>285</v>
+      </c>
+      <c r="F7" s="71" t="s">
         <v>190</v>
-      </c>
-      <c r="E7" s="60" t="s">
-        <v>191</v>
-      </c>
-      <c r="F7" s="71" t="s">
-        <v>192</v>
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="50"/>
@@ -27009,10 +27009,10 @@
       <c r="B8" s="93"/>
       <c r="C8" s="93"/>
       <c r="D8" s="60" t="s">
-        <v>193</v>
+        <v>287</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="F8" s="49"/>
       <c r="G8" s="49"/>
@@ -27022,10 +27022,10 @@
       <c r="K8" s="50"/>
       <c r="L8" s="51"/>
       <c r="M8" s="52" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="N8" s="52" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="O8" s="52"/>
       <c r="P8" s="52"/>
@@ -27074,19 +27074,19 @@
         <v>114</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C11" s="125" t="s">
         <v>189</v>
       </c>
       <c r="D11" s="60" t="s">
-        <v>198</v>
+        <v>288</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>191</v>
+        <v>285</v>
       </c>
       <c r="F11" s="71" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G11" s="50"/>
       <c r="H11" s="50"/>
@@ -27105,10 +27105,10 @@
       <c r="B12" s="93"/>
       <c r="C12" s="93"/>
       <c r="D12" s="60" t="s">
-        <v>193</v>
+        <v>287</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="F12" s="49"/>
       <c r="G12" s="49"/>
@@ -27118,10 +27118,10 @@
       <c r="K12" s="50"/>
       <c r="L12" s="51"/>
       <c r="M12" s="52" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="N12" s="52" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="O12" s="53"/>
       <c r="P12" s="53"/>
@@ -28859,7 +28859,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="123" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="C3" s="120"/>
       <c r="D3" s="121"/>
@@ -29856,7 +29856,7 @@
         <v>135</v>
       </c>
       <c r="C7" s="93" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>137</v>
@@ -30113,7 +30113,7 @@
         <v>140</v>
       </c>
       <c r="E8" s="74" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="F8" s="71" t="s">
         <v>141</v>
@@ -31356,7 +31356,7 @@
         <v>148</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="D13" s="60" t="s">
         <v>137</v>
@@ -31613,7 +31613,7 @@
         <v>140</v>
       </c>
       <c r="E14" s="74" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="F14" s="71" t="s">
         <v>141</v>
@@ -33113,7 +33113,7 @@
         <v>140</v>
       </c>
       <c r="E20" s="74" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="F20" s="71" t="s">
         <v>141</v>
@@ -36942,7 +36942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -37015,10 +37015,10 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="87" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="B3" s="131" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="C3" s="114"/>
       <c r="D3" s="115"/>
@@ -37041,7 +37041,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="132" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="C4" s="117"/>
       <c r="D4" s="118"/>
@@ -37112,20 +37112,20 @@
         <v>163</v>
       </c>
       <c r="B7" s="134" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="C7" s="135" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D7" s="136" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="E7" s="136" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="F7" s="150" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="G7" s="138"/>
       <c r="H7" s="138"/>
@@ -37134,7 +37134,7 @@
       <c r="K7" s="138"/>
       <c r="L7" s="51"/>
       <c r="M7" s="139" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="N7" s="139"/>
       <c r="O7" s="139"/>
@@ -37203,34 +37203,34 @@
         <v>114</v>
       </c>
       <c r="B11" s="134" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C11" s="135" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D11" s="136" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="E11" s="136" t="str">
         <f>E7</f>
         <v>O sistema informará conforme dados de saída.</v>
       </c>
       <c r="F11" s="137" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="G11" s="150" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="H11" s="137" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="I11" s="137"/>
       <c r="J11" s="138"/>
       <c r="K11" s="138"/>
       <c r="L11" s="51"/>
       <c r="M11" s="139" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="N11" s="139"/>
       <c r="O11" s="139"/>
@@ -37299,7 +37299,7 @@
         <v>164</v>
       </c>
       <c r="B15" s="134" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="C15" s="135"/>
       <c r="D15" s="141" t="str">
@@ -37307,10 +37307,10 @@
         <v>Sistema informará Conforme dados de entrada.</v>
       </c>
       <c r="E15" s="136" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="F15" s="150" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="G15" s="137"/>
       <c r="H15" s="137"/>
@@ -37389,17 +37389,17 @@
         <v>165</v>
       </c>
       <c r="B19" s="134" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="C19" s="140" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D19" s="136" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="E19" s="136" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="F19" s="137"/>
       <c r="G19" s="137"/>
@@ -37419,10 +37419,10 @@
       <c r="B20" s="140"/>
       <c r="C20" s="140"/>
       <c r="D20" s="136" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="E20" s="136" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="F20" s="150"/>
       <c r="G20" s="150"/>
@@ -37480,17 +37480,17 @@
         <v>166</v>
       </c>
       <c r="B23" s="134" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="C23" s="140" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D23" s="136" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="E23" s="136" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="F23" s="137" t="str">
         <f>F11</f>
@@ -37509,7 +37509,7 @@
       <c r="K23" s="138"/>
       <c r="L23" s="51"/>
       <c r="M23" s="139" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="N23" s="139"/>
       <c r="O23" s="139"/>
@@ -37578,7 +37578,7 @@
         <v>167</v>
       </c>
       <c r="B27" s="134" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="C27" s="140" t="str">
         <f>B3</f>
@@ -37593,7 +37593,7 @@
         <v>o sistema informará uma mensagem Conforme dados de saída.</v>
       </c>
       <c r="F27" s="150" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="G27" s="138"/>
       <c r="H27" s="138"/>
@@ -37602,7 +37602,7 @@
       <c r="K27" s="138"/>
       <c r="L27" s="51"/>
       <c r="M27" s="139" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="N27" s="139" t="str">
         <f>M11</f>
@@ -37674,7 +37674,7 @@
         <v>168</v>
       </c>
       <c r="B31" s="134" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="C31" s="140" t="str">
         <f>B3</f>
@@ -37689,10 +37689,10 @@
         <v>o sistema informará uma mensagem Conforme dados de saída.</v>
       </c>
       <c r="F31" s="150" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="G31" s="150" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="H31" s="150"/>
       <c r="I31" s="138"/>
@@ -37700,7 +37700,7 @@
       <c r="K31" s="138"/>
       <c r="L31" s="51"/>
       <c r="M31" s="139" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="N31" s="139"/>
       <c r="O31" s="139"/>
@@ -37769,7 +37769,7 @@
         <v>169</v>
       </c>
       <c r="B35" s="134" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="C35" s="140" t="str">
         <f>C31</f>
@@ -37784,7 +37784,7 @@
         <v>o sistema informará uma mensagem Conforme dados de saída.</v>
       </c>
       <c r="F35" s="150" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="G35" s="138"/>
       <c r="H35" s="138"/>
@@ -37793,7 +37793,7 @@
       <c r="K35" s="138"/>
       <c r="L35" s="51"/>
       <c r="M35" s="139" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="N35" s="139"/>
       <c r="O35" s="139"/>
@@ -37862,7 +37862,7 @@
         <v>170</v>
       </c>
       <c r="B39" s="134" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="C39" s="140" t="str">
         <f>C35</f>
@@ -37873,10 +37873,10 @@
         <v>Informar conforme dados de entrada.</v>
       </c>
       <c r="E39" s="136" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="F39" s="150" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="G39" s="138"/>
       <c r="H39" s="138"/>
@@ -37949,29 +37949,29 @@
     </row>
     <row r="43" spans="1:17" ht="153">
       <c r="A43" s="149" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="B43" s="134" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="C43" s="140" t="str">
         <f>C39</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D43" s="136" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="E43" s="136" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="F43" s="150" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="G43" s="150" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="H43" s="150" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="I43" s="138"/>
       <c r="J43" s="138"/>
@@ -38045,26 +38045,26 @@
         <v>172</v>
       </c>
       <c r="B47" s="134" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="C47" s="140" t="str">
         <f>C43</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
       <c r="D47" s="136" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="E47" s="136" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="F47" s="150" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="G47" s="150" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="H47" s="150" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="I47" s="138"/>
       <c r="J47" s="138"/>
@@ -38135,10 +38135,10 @@
     </row>
     <row r="51" spans="1:17" ht="114.75">
       <c r="A51" s="149" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="B51" s="134" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="C51" s="140" t="str">
         <f>C47</f>
@@ -38149,13 +38149,13 @@
         <v>Sistema informará Conforme dados de entrada.</v>
       </c>
       <c r="E51" s="136" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="F51" s="150" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="G51" s="150" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="H51" s="138"/>
       <c r="I51" s="138"/>

</xml_diff>

<commit_message>
atualizacao da merda que o bergson fez
</commit_message>
<xml_diff>
--- a/Requisitos/Template_Projeto.xlsx
+++ b/Requisitos/Template_Projeto.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" codeName="EstaPasta_de_trabalho" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="601" activeTab="1"/>
+    <workbookView xWindow="1215" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="601" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'UC002 - Efetuar pagamento SIB  '!$1:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'UC006 - comprar ações '!$1:$6</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2169,7 +2169,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="\C\T000"/>
@@ -3161,6 +3161,9 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3170,8 +3173,56 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -3209,57 +3260,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3283,6 +3283,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3308,56 +3356,8 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7249,7 +7249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7652,11 +7652,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan3"/>
   <dimension ref="A1:IH54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
@@ -7689,29 +7689,29 @@
       <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="133" t="s">
+      <c r="C1" s="153"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="150" t="s">
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="152"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="149"/>
       <c r="Q1" s="38"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -7943,33 +7943,33 @@
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="132" t="s">
+      <c r="C2" s="156"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="132" t="s">
+      <c r="G2" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="132" t="s">
+      <c r="H2" s="144" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="132" t="s">
+      <c r="I2" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="145" t="s">
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="141" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="157"/>
-      <c r="O2" s="157"/>
-      <c r="P2" s="157"/>
+      <c r="N2" s="133"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
       <c r="Q2" s="38"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -8198,26 +8198,26 @@
       <c r="IH2" s="1"/>
     </row>
     <row r="3" spans="1:242" s="6" customFormat="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="158" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158"/>
-      <c r="P3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -8446,22 +8446,22 @@
       <c r="IH3" s="1"/>
     </row>
     <row r="4" spans="1:242" s="6" customFormat="1">
-      <c r="A4" s="161"/>
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="149"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="153"/>
+      <c r="D4" s="154"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
+      <c r="I4" s="144"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="146"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="135"/>
       <c r="Q4" s="38"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -9188,13 +9188,13 @@
       <c r="IH6" s="1"/>
     </row>
     <row r="7" spans="1:242" s="9" customFormat="1" ht="63.75">
-      <c r="A7" s="129" t="s">
+      <c r="A7" s="130" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="131" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="61" t="s">
@@ -9442,9 +9442,9 @@
       <c r="IH7" s="13"/>
     </row>
     <row r="8" spans="1:242" s="9" customFormat="1" ht="72.75" customHeight="1">
-      <c r="A8" s="129"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
+      <c r="A8" s="130"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="62" t="s">
         <v>24</v>
       </c>
@@ -9700,9 +9700,9 @@
       <c r="IH8" s="13"/>
     </row>
     <row r="9" spans="1:242" s="9" customFormat="1" ht="44.1" customHeight="1" thickBot="1">
-      <c r="A9" s="129"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
       <c r="D9" s="48"/>
       <c r="E9" s="48"/>
       <c r="F9" s="50"/>
@@ -10188,13 +10188,13 @@
       <c r="IH10"/>
     </row>
     <row r="11" spans="1:242" s="9" customFormat="1" ht="63.75">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="131" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="60" t="s">
@@ -10442,9 +10442,9 @@
       <c r="IH11" s="13"/>
     </row>
     <row r="12" spans="1:242" s="9" customFormat="1" ht="63.75">
-      <c r="A12" s="129"/>
-      <c r="B12" s="131"/>
-      <c r="C12" s="131"/>
+      <c r="A12" s="130"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="132"/>
       <c r="D12" s="60" t="s">
         <v>77</v>
       </c>
@@ -10700,9 +10700,9 @@
       <c r="IH12" s="13"/>
     </row>
     <row r="13" spans="1:242" s="9" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A13" s="129"/>
-      <c r="B13" s="131"/>
-      <c r="C13" s="131"/>
+      <c r="A13" s="130"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="132"/>
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
       <c r="F13" s="50"/>
@@ -11188,13 +11188,13 @@
       <c r="IH14"/>
     </row>
     <row r="15" spans="1:242" s="9" customFormat="1" ht="63.75">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="130" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="131" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="131" t="s">
+      <c r="C15" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="60" t="s">
@@ -11442,9 +11442,9 @@
       <c r="IH15" s="13"/>
     </row>
     <row r="16" spans="1:242" s="9" customFormat="1" ht="63.75">
-      <c r="A16" s="129"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
+      <c r="A16" s="130"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
       <c r="D16" s="60" t="s">
         <v>73</v>
       </c>
@@ -11700,9 +11700,9 @@
       <c r="IH16" s="13"/>
     </row>
     <row r="17" spans="1:242" s="9" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A17" s="129"/>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
+      <c r="A17" s="130"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="132"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
       <c r="F17" s="50"/>
@@ -12188,13 +12188,13 @@
       <c r="IH18"/>
     </row>
     <row r="19" spans="1:242" s="9" customFormat="1" ht="63.75">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="129" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="130" t="s">
+      <c r="B19" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="131" t="s">
+      <c r="C19" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="60" t="s">
@@ -12442,9 +12442,9 @@
       <c r="IH19" s="13"/>
     </row>
     <row r="20" spans="1:242" s="9" customFormat="1" ht="169.5" customHeight="1">
-      <c r="A20" s="129"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
+      <c r="A20" s="130"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="132"/>
       <c r="D20" s="60" t="s">
         <v>70</v>
       </c>
@@ -12700,9 +12700,9 @@
       <c r="IH20" s="13"/>
     </row>
     <row r="21" spans="1:242" s="9" customFormat="1" ht="74.099999999999994" customHeight="1" thickBot="1">
-      <c r="A21" s="129"/>
-      <c r="B21" s="131"/>
-      <c r="C21" s="131"/>
+      <c r="A21" s="130"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="132"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
       <c r="F21" s="50"/>
@@ -13188,13 +13188,13 @@
       <c r="IH22"/>
     </row>
     <row r="23" spans="1:242" ht="60" customHeight="1">
-      <c r="A23" s="156" t="s">
+      <c r="A23" s="129" t="s">
         <v>159</v>
       </c>
-      <c r="B23" s="130" t="s">
+      <c r="B23" s="131" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="131" t="s">
+      <c r="C23" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="60" t="s">
@@ -13217,9 +13217,9 @@
       <c r="Q23" s="38"/>
     </row>
     <row r="24" spans="1:242" ht="89.25">
-      <c r="A24" s="129"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
+      <c r="A24" s="130"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="132"/>
       <c r="D24" s="60" t="s">
         <v>66</v>
       </c>
@@ -13250,9 +13250,9 @@
       <c r="Q24" s="38"/>
     </row>
     <row r="25" spans="1:242" ht="13.5" thickBot="1">
-      <c r="A25" s="129"/>
-      <c r="B25" s="131"/>
-      <c r="C25" s="131"/>
+      <c r="A25" s="130"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
       <c r="D25" s="48"/>
       <c r="E25" s="48"/>
       <c r="F25" s="50"/>
@@ -13288,13 +13288,13 @@
       <c r="Q26" s="58"/>
     </row>
     <row r="27" spans="1:242" ht="63.75">
-      <c r="A27" s="156" t="s">
+      <c r="A27" s="129" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="130" t="s">
+      <c r="B27" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="131" t="s">
+      <c r="C27" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="60" t="s">
@@ -13317,9 +13317,9 @@
       <c r="Q27" s="38"/>
     </row>
     <row r="28" spans="1:242" ht="63.75">
-      <c r="A28" s="129"/>
-      <c r="B28" s="131"/>
-      <c r="C28" s="131"/>
+      <c r="A28" s="130"/>
+      <c r="B28" s="132"/>
+      <c r="C28" s="132"/>
       <c r="D28" s="48" t="s">
         <v>30</v>
       </c>
@@ -13350,9 +13350,9 @@
       <c r="Q28" s="38"/>
     </row>
     <row r="29" spans="1:242" ht="13.5" thickBot="1">
-      <c r="A29" s="129"/>
-      <c r="B29" s="131"/>
-      <c r="C29" s="131"/>
+      <c r="A29" s="130"/>
+      <c r="B29" s="132"/>
+      <c r="C29" s="132"/>
       <c r="D29" s="48"/>
       <c r="E29" s="48"/>
       <c r="F29" s="50"/>
@@ -13388,13 +13388,13 @@
       <c r="Q30" s="58"/>
     </row>
     <row r="31" spans="1:242" ht="60.75" customHeight="1">
-      <c r="A31" s="156" t="s">
+      <c r="A31" s="129" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="130" t="s">
+      <c r="B31" s="131" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="60" t="s">
@@ -13417,9 +13417,9 @@
       <c r="Q31" s="38"/>
     </row>
     <row r="32" spans="1:242" ht="63.75">
-      <c r="A32" s="129"/>
-      <c r="B32" s="131"/>
-      <c r="C32" s="131"/>
+      <c r="A32" s="130"/>
+      <c r="B32" s="132"/>
+      <c r="C32" s="132"/>
       <c r="D32" s="60" t="s">
         <v>60</v>
       </c>
@@ -13450,9 +13450,9 @@
       <c r="Q32" s="38"/>
     </row>
     <row r="33" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A33" s="129"/>
-      <c r="B33" s="131"/>
-      <c r="C33" s="131"/>
+      <c r="A33" s="130"/>
+      <c r="B33" s="132"/>
+      <c r="C33" s="132"/>
       <c r="D33" s="48"/>
       <c r="E33" s="48"/>
       <c r="F33" s="50"/>
@@ -13488,13 +13488,13 @@
       <c r="Q34" s="58"/>
     </row>
     <row r="35" spans="1:17" ht="63.75">
-      <c r="A35" s="156" t="s">
+      <c r="A35" s="129" t="s">
         <v>162</v>
       </c>
-      <c r="B35" s="130" t="s">
+      <c r="B35" s="131" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="131" t="s">
+      <c r="C35" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="60" t="s">
@@ -13517,9 +13517,9 @@
       <c r="Q35" s="38"/>
     </row>
     <row r="36" spans="1:17" ht="89.25">
-      <c r="A36" s="129"/>
-      <c r="B36" s="131"/>
-      <c r="C36" s="131"/>
+      <c r="A36" s="130"/>
+      <c r="B36" s="132"/>
+      <c r="C36" s="132"/>
       <c r="D36" s="60" t="s">
         <v>54</v>
       </c>
@@ -13550,9 +13550,9 @@
       <c r="Q36" s="38"/>
     </row>
     <row r="37" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A37" s="129"/>
-      <c r="B37" s="131"/>
-      <c r="C37" s="131"/>
+      <c r="A37" s="130"/>
+      <c r="B37" s="132"/>
+      <c r="C37" s="132"/>
       <c r="D37" s="48"/>
       <c r="E37" s="48"/>
       <c r="F37" s="50"/>
@@ -13588,13 +13588,13 @@
       <c r="Q38" s="58"/>
     </row>
     <row r="39" spans="1:17" ht="63.75">
-      <c r="A39" s="156" t="s">
+      <c r="A39" s="129" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="130" t="s">
+      <c r="B39" s="131" t="s">
         <v>201</v>
       </c>
-      <c r="C39" s="131" t="s">
+      <c r="C39" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D39" s="60" t="s">
@@ -13617,9 +13617,9 @@
       <c r="Q39" s="38"/>
     </row>
     <row r="40" spans="1:17" ht="178.5">
-      <c r="A40" s="129"/>
-      <c r="B40" s="131"/>
-      <c r="C40" s="131"/>
+      <c r="A40" s="130"/>
+      <c r="B40" s="132"/>
+      <c r="C40" s="132"/>
       <c r="D40" s="60" t="s">
         <v>202</v>
       </c>
@@ -13650,9 +13650,9 @@
       <c r="Q40" s="38"/>
     </row>
     <row r="41" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A41" s="129"/>
-      <c r="B41" s="131"/>
-      <c r="C41" s="131"/>
+      <c r="A41" s="130"/>
+      <c r="B41" s="132"/>
+      <c r="C41" s="132"/>
       <c r="D41" s="48"/>
       <c r="E41" s="48"/>
       <c r="F41" s="50"/>
@@ -13688,13 +13688,13 @@
       <c r="Q42" s="58"/>
     </row>
     <row r="43" spans="1:17" ht="63.75">
-      <c r="A43" s="156" t="s">
+      <c r="A43" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="B43" s="130" t="s">
+      <c r="B43" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="131" t="s">
+      <c r="C43" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D43" s="60" t="s">
@@ -13717,9 +13717,9 @@
       <c r="Q43" s="38"/>
     </row>
     <row r="44" spans="1:17" ht="102">
-      <c r="A44" s="129"/>
-      <c r="B44" s="131"/>
-      <c r="C44" s="131"/>
+      <c r="A44" s="130"/>
+      <c r="B44" s="132"/>
+      <c r="C44" s="132"/>
       <c r="D44" s="60" t="s">
         <v>49</v>
       </c>
@@ -13750,9 +13750,9 @@
       <c r="Q44" s="38"/>
     </row>
     <row r="45" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A45" s="129"/>
-      <c r="B45" s="131"/>
-      <c r="C45" s="131"/>
+      <c r="A45" s="130"/>
+      <c r="B45" s="132"/>
+      <c r="C45" s="132"/>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
       <c r="F45" s="50"/>
@@ -13788,13 +13788,13 @@
       <c r="Q46" s="58"/>
     </row>
     <row r="47" spans="1:17" ht="63.75">
-      <c r="A47" s="156" t="s">
+      <c r="A47" s="129" t="s">
         <v>165</v>
       </c>
-      <c r="B47" s="130" t="s">
+      <c r="B47" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="131" t="s">
+      <c r="C47" s="132" t="s">
         <v>25</v>
       </c>
       <c r="D47" s="60" t="s">
@@ -13817,9 +13817,9 @@
       <c r="Q47" s="38"/>
     </row>
     <row r="48" spans="1:17" ht="153">
-      <c r="A48" s="129"/>
-      <c r="B48" s="131"/>
-      <c r="C48" s="131"/>
+      <c r="A48" s="130"/>
+      <c r="B48" s="132"/>
+      <c r="C48" s="132"/>
       <c r="D48" s="60" t="s">
         <v>205</v>
       </c>
@@ -13850,9 +13850,9 @@
       <c r="Q48" s="38"/>
     </row>
     <row r="49" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A49" s="129"/>
-      <c r="B49" s="131"/>
-      <c r="C49" s="131"/>
+      <c r="A49" s="130"/>
+      <c r="B49" s="132"/>
+      <c r="C49" s="132"/>
       <c r="D49" s="48"/>
       <c r="E49" s="48"/>
       <c r="F49" s="50"/>
@@ -13969,24 +13969,23 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="L1:L4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="J2:J4"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
@@ -14003,23 +14002,24 @@
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="L1:L4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="G6:K6 M6:P9 F9">
@@ -15115,7 +15115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IH29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15157,24 +15157,24 @@
       </c>
       <c r="C1" s="65"/>
       <c r="D1" s="66"/>
-      <c r="E1" s="133" t="s">
+      <c r="E1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="150" t="s">
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="152"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="149"/>
       <c r="Q1" s="38"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -15411,30 +15411,30 @@
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="69"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="153" t="s">
+      <c r="E2" s="150"/>
+      <c r="F2" s="136" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="153" t="s">
+      <c r="G2" s="136" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="153" t="s">
+      <c r="H2" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="145" t="s">
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="141" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="157" t="s">
+      <c r="N2" s="133" t="s">
         <v>88</v>
       </c>
-      <c r="O2" s="157" t="s">
+      <c r="O2" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="P2" s="157"/>
+      <c r="P2" s="133"/>
       <c r="Q2" s="38"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -15663,26 +15663,26 @@
       <c r="IH2" s="1"/>
     </row>
     <row r="3" spans="1:242" s="6" customFormat="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="158" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158"/>
-      <c r="P3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -15911,22 +15911,22 @@
       <c r="IH3" s="1"/>
     </row>
     <row r="4" spans="1:242" s="6" customFormat="1" ht="33" customHeight="1">
-      <c r="A4" s="161"/>
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="149"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="153"/>
+      <c r="D4" s="154"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="146"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="135"/>
       <c r="Q4" s="38"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -16653,13 +16653,13 @@
       <c r="IH6" s="1"/>
     </row>
     <row r="7" spans="1:242" s="9" customFormat="1" ht="38.25">
-      <c r="A7" s="129">
+      <c r="A7" s="130">
         <v>1</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="131" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="60" t="s">
@@ -16907,9 +16907,9 @@
       <c r="IH7" s="13"/>
     </row>
     <row r="8" spans="1:242" s="9" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A8" s="129"/>
-      <c r="B8" s="130"/>
-      <c r="C8" s="131"/>
+      <c r="A8" s="130"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="60" t="s">
         <v>96</v>
       </c>
@@ -17157,9 +17157,9 @@
       <c r="IH8" s="13"/>
     </row>
     <row r="9" spans="1:242" s="9" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A9" s="129"/>
-      <c r="B9" s="130"/>
-      <c r="C9" s="131"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="132"/>
       <c r="D9" s="60"/>
       <c r="E9" s="60" t="s">
         <v>99</v>
@@ -17403,9 +17403,9 @@
       <c r="IH9" s="13"/>
     </row>
     <row r="10" spans="1:242" s="9" customFormat="1" ht="63.75">
-      <c r="A10" s="129"/>
-      <c r="B10" s="131"/>
-      <c r="C10" s="131"/>
+      <c r="A10" s="130"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="132"/>
       <c r="D10" s="60" t="s">
         <v>100</v>
       </c>
@@ -17653,9 +17653,9 @@
       <c r="IH10" s="13"/>
     </row>
     <row r="11" spans="1:242" s="9" customFormat="1" ht="77.25" thickBot="1">
-      <c r="A11" s="129"/>
-      <c r="B11" s="131"/>
-      <c r="C11" s="131"/>
+      <c r="A11" s="130"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
       <c r="D11" s="60" t="s">
         <v>103</v>
       </c>
@@ -18151,13 +18151,13 @@
       <c r="IH12"/>
     </row>
     <row r="13" spans="1:242" s="9" customFormat="1" ht="38.25">
-      <c r="A13" s="129" t="s">
+      <c r="A13" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="130" t="s">
+      <c r="B13" s="131" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="131" t="s">
+      <c r="C13" s="132" t="s">
         <v>93</v>
       </c>
       <c r="D13" s="60" t="s">
@@ -18405,9 +18405,9 @@
       <c r="IH13" s="13"/>
     </row>
     <row r="14" spans="1:242" s="9" customFormat="1" ht="25.5">
-      <c r="A14" s="129"/>
-      <c r="B14" s="130"/>
-      <c r="C14" s="131"/>
+      <c r="A14" s="130"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="60" t="s">
         <v>96</v>
       </c>
@@ -18655,9 +18655,9 @@
       <c r="IH14" s="13"/>
     </row>
     <row r="15" spans="1:242" s="9" customFormat="1" ht="38.25">
-      <c r="A15" s="129"/>
-      <c r="B15" s="130"/>
-      <c r="C15" s="131"/>
+      <c r="A15" s="130"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="132"/>
       <c r="D15" s="60"/>
       <c r="E15" s="60" t="s">
         <v>99</v>
@@ -18901,9 +18901,9 @@
       <c r="IH15" s="13"/>
     </row>
     <row r="16" spans="1:242" s="9" customFormat="1" ht="38.25">
-      <c r="A16" s="129"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
+      <c r="A16" s="130"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
       <c r="D16" s="60" t="s">
         <v>111</v>
       </c>
@@ -19151,9 +19151,9 @@
       <c r="IH16" s="13"/>
     </row>
     <row r="17" spans="1:242" s="9" customFormat="1" ht="81.75" customHeight="1" thickBot="1">
-      <c r="A17" s="129"/>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
+      <c r="A17" s="130"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="132"/>
       <c r="D17" s="60" t="s">
         <v>103</v>
       </c>
@@ -19649,13 +19649,13 @@
       <c r="IH18"/>
     </row>
     <row r="19" spans="1:242" s="9" customFormat="1" ht="38.25">
-      <c r="A19" s="129">
+      <c r="A19" s="130">
         <v>3</v>
       </c>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="132" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="131" t="s">
+      <c r="C19" s="132" t="s">
         <v>93</v>
       </c>
       <c r="D19" s="60" t="s">
@@ -19903,9 +19903,9 @@
       <c r="IH19" s="13"/>
     </row>
     <row r="20" spans="1:242" s="9" customFormat="1" ht="25.5">
-      <c r="A20" s="129"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
+      <c r="A20" s="130"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="132"/>
       <c r="D20" s="60" t="s">
         <v>96</v>
       </c>
@@ -20153,9 +20153,9 @@
       <c r="IH20" s="13"/>
     </row>
     <row r="21" spans="1:242" s="9" customFormat="1" ht="25.5">
-      <c r="A21" s="129"/>
-      <c r="B21" s="131"/>
-      <c r="C21" s="131"/>
+      <c r="A21" s="130"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="132"/>
       <c r="D21" s="48"/>
       <c r="E21" s="60" t="s">
         <v>116</v>
@@ -20399,9 +20399,9 @@
       <c r="IH21" s="13"/>
     </row>
     <row r="22" spans="1:242" s="9" customFormat="1" ht="77.25" thickBot="1">
-      <c r="A22" s="129"/>
-      <c r="B22" s="131"/>
-      <c r="C22" s="131"/>
+      <c r="A22" s="130"/>
+      <c r="B22" s="132"/>
+      <c r="C22" s="132"/>
       <c r="D22" s="48"/>
       <c r="E22" s="60" t="s">
         <v>117</v>
@@ -20891,13 +20891,13 @@
       <c r="IH23"/>
     </row>
     <row r="24" spans="1:242" s="9" customFormat="1" ht="38.25">
-      <c r="A24" s="129">
+      <c r="A24" s="130">
         <v>4</v>
       </c>
-      <c r="B24" s="131" t="s">
+      <c r="B24" s="132" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="131" t="s">
+      <c r="C24" s="132" t="s">
         <v>93</v>
       </c>
       <c r="D24" s="60" t="s">
@@ -21147,9 +21147,9 @@
       <c r="IH24" s="13"/>
     </row>
     <row r="25" spans="1:242" s="9" customFormat="1" ht="25.5">
-      <c r="A25" s="129"/>
-      <c r="B25" s="131"/>
-      <c r="C25" s="131"/>
+      <c r="A25" s="130"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
       <c r="D25" s="60" t="s">
         <v>96</v>
       </c>
@@ -21397,9 +21397,9 @@
       <c r="IH25" s="13"/>
     </row>
     <row r="26" spans="1:242" s="9" customFormat="1" ht="38.25">
-      <c r="A26" s="129"/>
-      <c r="B26" s="131"/>
-      <c r="C26" s="131"/>
+      <c r="A26" s="130"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="132"/>
       <c r="D26" s="60"/>
       <c r="E26" s="60" t="s">
         <v>99</v>
@@ -21643,9 +21643,9 @@
       <c r="IH26" s="13"/>
     </row>
     <row r="27" spans="1:242" s="9" customFormat="1" ht="38.25">
-      <c r="A27" s="129"/>
-      <c r="B27" s="131"/>
-      <c r="C27" s="131"/>
+      <c r="A27" s="130"/>
+      <c r="B27" s="132"/>
+      <c r="C27" s="132"/>
       <c r="D27" s="60" t="s">
         <v>111</v>
       </c>
@@ -21893,9 +21893,9 @@
       <c r="IH27" s="13"/>
     </row>
     <row r="28" spans="1:242" s="9" customFormat="1" ht="84.75" customHeight="1" thickBot="1">
-      <c r="A28" s="129"/>
-      <c r="B28" s="131"/>
-      <c r="C28" s="131"/>
+      <c r="A28" s="130"/>
+      <c r="B28" s="132"/>
+      <c r="C28" s="132"/>
       <c r="D28" s="48"/>
       <c r="E28" s="60" t="s">
         <v>122</v>
@@ -22390,6 +22390,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C13:C17"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
@@ -22406,18 +22418,6 @@
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="J2:J4"/>
     <mergeCell ref="K2:K4"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="C24:C28"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K6 F7:F11 M6:P11">
     <cfRule type="cellIs" priority="103" stopIfTrue="1" operator="equal">
@@ -22844,7 +22844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22871,102 +22871,102 @@
       <c r="A1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="133" t="s">
+      <c r="C1" s="153"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="150" t="s">
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="152"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="149"/>
       <c r="Q1" s="38"/>
     </row>
     <row r="2" spans="1:17" ht="27.75" customHeight="1">
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="153" t="s">
+      <c r="C2" s="156"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="136" t="s">
         <v>186</v>
       </c>
-      <c r="G2" s="153" t="s">
+      <c r="G2" s="136" t="s">
         <v>187</v>
       </c>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="145" t="s">
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="141" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="157" t="s">
+      <c r="N2" s="133" t="s">
         <v>176</v>
       </c>
-      <c r="O2" s="157"/>
-      <c r="P2" s="157"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
       <c r="Q2" s="38"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="139" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="162" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158"/>
-      <c r="P3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="Q3" s="38"/>
     </row>
     <row r="4" spans="1:17" ht="17.25" customHeight="1">
-      <c r="A4" s="161"/>
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="149"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="153"/>
+      <c r="D4" s="154"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="146"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="135"/>
       <c r="Q4" s="38"/>
     </row>
     <row r="5" spans="1:17">
@@ -23018,13 +23018,13 @@
       <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:17" ht="80.25" customHeight="1">
-      <c r="A7" s="129" t="s">
+      <c r="A7" s="130" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="131" t="s">
         <v>189</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="131" t="s">
         <v>190</v>
       </c>
       <c r="D7" s="60" t="s">
@@ -23047,9 +23047,9 @@
       <c r="Q7" s="38"/>
     </row>
     <row r="8" spans="1:17" ht="78" customHeight="1">
-      <c r="A8" s="129"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
+      <c r="A8" s="130"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="60" t="s">
         <v>250</v>
       </c>
@@ -23076,9 +23076,9 @@
       <c r="Q8" s="38"/>
     </row>
     <row r="9" spans="1:17" ht="124.5" customHeight="1" thickBot="1">
-      <c r="A9" s="129"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
       <c r="D9" s="60" t="s">
         <v>195</v>
       </c>
@@ -23120,13 +23120,13 @@
       <c r="Q10" s="58"/>
     </row>
     <row r="11" spans="1:17" ht="86.25" customHeight="1">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="131" t="s">
         <v>196</v>
       </c>
-      <c r="C11" s="130" t="s">
+      <c r="C11" s="131" t="s">
         <v>190</v>
       </c>
       <c r="D11" s="60" t="s">
@@ -23149,9 +23149,9 @@
       <c r="Q11" s="38"/>
     </row>
     <row r="12" spans="1:17" ht="98.25" customHeight="1">
-      <c r="A12" s="129"/>
-      <c r="B12" s="131"/>
-      <c r="C12" s="131"/>
+      <c r="A12" s="130"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="132"/>
       <c r="D12" s="60" t="s">
         <v>250</v>
       </c>
@@ -23178,9 +23178,9 @@
       <c r="Q12" s="38"/>
     </row>
     <row r="13" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A13" s="129"/>
-      <c r="B13" s="131"/>
-      <c r="C13" s="131"/>
+      <c r="A13" s="130"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="132"/>
       <c r="D13" s="60"/>
       <c r="E13" s="60"/>
       <c r="F13" s="71"/>
@@ -23216,13 +23216,13 @@
       <c r="Q14" s="58"/>
     </row>
     <row r="15" spans="1:17" ht="86.25" customHeight="1">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="130" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="131" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="131" t="s">
         <v>190</v>
       </c>
       <c r="D15" s="60" t="s">
@@ -23245,9 +23245,9 @@
       <c r="Q15" s="38"/>
     </row>
     <row r="16" spans="1:17" ht="97.5" customHeight="1">
-      <c r="A16" s="129"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
+      <c r="A16" s="130"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
       <c r="D16" s="60" t="s">
         <v>250</v>
       </c>
@@ -23274,9 +23274,9 @@
       <c r="Q16" s="38"/>
     </row>
     <row r="17" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A17" s="129"/>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
+      <c r="A17" s="130"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="132"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
       <c r="F17" s="50"/>
@@ -23312,13 +23312,13 @@
       <c r="Q18" s="58"/>
     </row>
     <row r="19" spans="1:17" ht="111.75" customHeight="1">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="130" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="130" t="s">
+      <c r="B19" s="131" t="s">
         <v>200</v>
       </c>
-      <c r="C19" s="130" t="s">
+      <c r="C19" s="131" t="s">
         <v>190</v>
       </c>
       <c r="D19" s="60" t="s">
@@ -23345,9 +23345,9 @@
       <c r="Q19" s="38"/>
     </row>
     <row r="20" spans="1:17" ht="99" customHeight="1">
-      <c r="A20" s="129"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
+      <c r="A20" s="130"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="132"/>
       <c r="D20" s="60" t="s">
         <v>250</v>
       </c>
@@ -23372,9 +23372,9 @@
       <c r="Q20" s="38"/>
     </row>
     <row r="21" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A21" s="129"/>
-      <c r="B21" s="131"/>
-      <c r="C21" s="131"/>
+      <c r="A21" s="130"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="132"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
       <c r="F21" s="50"/>
@@ -23411,22 +23411,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
@@ -23441,6 +23425,22 @@
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F9 G6:K6 M6:P9">
     <cfRule type="cellIs" priority="205" stopIfTrue="1" operator="equal">
@@ -24274,7 +24274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24300,81 +24300,81 @@
       <c r="A1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="133" t="s">
+      <c r="C1" s="153"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="150" t="s">
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="152"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="149"/>
       <c r="Q1" s="38"/>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1">
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="153" t="s">
+      <c r="C2" s="156"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="136" t="s">
         <v>175</v>
       </c>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="145" t="s">
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="141" t="s">
         <v>176</v>
       </c>
-      <c r="N2" s="157" t="s">
+      <c r="N2" s="133" t="s">
         <v>177</v>
       </c>
-      <c r="O2" s="157"/>
-      <c r="P2" s="157"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
       <c r="Q2" s="38"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="139" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="166" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158"/>
-      <c r="P3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="Q3" s="38"/>
     </row>
     <row r="4" spans="1:17" ht="41.25" customHeight="1">
@@ -24382,18 +24382,18 @@
       <c r="B4" s="167"/>
       <c r="C4" s="168"/>
       <c r="D4" s="169"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
-      <c r="H4" s="154"/>
-      <c r="I4" s="154"/>
-      <c r="J4" s="154"/>
-      <c r="K4" s="154"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="146"/>
-      <c r="N4" s="158"/>
-      <c r="O4" s="158"/>
-      <c r="P4" s="158"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="137"/>
+      <c r="H4" s="137"/>
+      <c r="I4" s="137"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="137"/>
+      <c r="L4" s="145"/>
+      <c r="M4" s="142"/>
+      <c r="N4" s="134"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
       <c r="Q4" s="38"/>
     </row>
     <row r="5" spans="1:17">
@@ -24448,7 +24448,7 @@
       <c r="A7" s="163" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="131" t="s">
         <v>179</v>
       </c>
       <c r="C7" s="164" t="s">
@@ -24476,9 +24476,9 @@
       <c r="Q7" s="38"/>
     </row>
     <row r="8" spans="1:17" ht="91.5" customHeight="1" thickBot="1">
-      <c r="A8" s="129"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
+      <c r="A8" s="130"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="60" t="s">
         <v>254</v>
       </c>
@@ -24503,9 +24503,9 @@
       <c r="Q8" s="38"/>
     </row>
     <row r="9" spans="1:17" ht="13.5" hidden="1" thickBot="1">
-      <c r="A9" s="129"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
       <c r="D9" s="48"/>
       <c r="E9" s="48"/>
       <c r="F9" s="50"/>
@@ -24544,7 +24544,7 @@
       <c r="A11" s="163" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="131" t="s">
         <v>184</v>
       </c>
       <c r="C11" s="164" t="s">
@@ -24572,9 +24572,9 @@
       <c r="Q11" s="38"/>
     </row>
     <row r="12" spans="1:17" ht="99.75" customHeight="1">
-      <c r="A12" s="129"/>
-      <c r="B12" s="131"/>
-      <c r="C12" s="131"/>
+      <c r="A12" s="130"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="132"/>
       <c r="D12" s="60" t="s">
         <v>254</v>
       </c>
@@ -24599,9 +24599,9 @@
       <c r="Q12" s="38"/>
     </row>
     <row r="13" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A13" s="129"/>
-      <c r="B13" s="131"/>
-      <c r="C13" s="131"/>
+      <c r="A13" s="130"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="132"/>
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
       <c r="F13" s="50"/>
@@ -24638,16 +24638,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
@@ -24662,6 +24652,16 @@
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F9 G6:K6 M6:P9">
     <cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal">
@@ -24780,7 +24780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24807,98 +24807,98 @@
       <c r="A1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="136"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="133" t="s">
+      <c r="C1" s="153"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="150" t="s">
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="152"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="149"/>
       <c r="Q1" s="38"/>
     </row>
     <row r="2" spans="1:17" ht="23.25" customHeight="1">
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="155" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="153" t="s">
+      <c r="C2" s="156"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="136" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="145" t="s">
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="141" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="157"/>
-      <c r="O2" s="157"/>
-      <c r="P2" s="157"/>
+      <c r="N2" s="133"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
       <c r="Q2" s="38"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="158" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158"/>
-      <c r="P3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
       <c r="Q3" s="38"/>
     </row>
     <row r="4" spans="1:17" ht="20.25" customHeight="1">
-      <c r="A4" s="161"/>
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="149"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="153"/>
+      <c r="D4" s="154"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="146"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="135"/>
       <c r="Q4" s="38"/>
     </row>
     <row r="5" spans="1:17">
@@ -24950,13 +24950,13 @@
       <c r="Q6" s="42"/>
     </row>
     <row r="7" spans="1:17" ht="89.25" customHeight="1">
-      <c r="A7" s="129" t="s">
+      <c r="A7" s="130" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="132" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>168</v>
       </c>
       <c r="D7" s="48" t="s">
@@ -24981,9 +24981,9 @@
       <c r="Q7" s="38"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="129"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="131"/>
+      <c r="A8" s="130"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="48"/>
       <c r="E8" s="48"/>
       <c r="F8" s="49"/>
@@ -25000,9 +25000,9 @@
       <c r="Q8" s="38"/>
     </row>
     <row r="9" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A9" s="129"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
       <c r="D9" s="48"/>
       <c r="E9" s="48"/>
       <c r="F9" s="50"/>
@@ -25038,13 +25038,13 @@
       <c r="Q10" s="58"/>
     </row>
     <row r="11" spans="1:17" ht="104.25" customHeight="1">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="131" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="132" t="s">
         <v>166</v>
       </c>
       <c r="D11" s="48" t="s">
@@ -25071,9 +25071,9 @@
       <c r="Q11" s="38"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="129"/>
-      <c r="B12" s="131"/>
-      <c r="C12" s="131"/>
+      <c r="A12" s="130"/>
+      <c r="B12" s="132"/>
+      <c r="C12" s="132"/>
       <c r="D12" s="48"/>
       <c r="E12" s="48"/>
       <c r="F12" s="49"/>
@@ -25090,9 +25090,9 @@
       <c r="Q12" s="38"/>
     </row>
     <row r="13" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A13" s="129"/>
-      <c r="B13" s="131"/>
-      <c r="C13" s="131"/>
+      <c r="A13" s="130"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="132"/>
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
       <c r="F13" s="50"/>
@@ -25128,13 +25128,13 @@
       <c r="Q14" s="58"/>
     </row>
     <row r="15" spans="1:17" ht="66" customHeight="1">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="130" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="131" t="s">
         <v>173</v>
       </c>
-      <c r="C15" s="131" t="s">
+      <c r="C15" s="132" t="s">
         <v>166</v>
       </c>
       <c r="D15" s="48" t="s">
@@ -25161,9 +25161,9 @@
       <c r="Q15" s="38"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="129"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
+      <c r="A16" s="130"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
       <c r="F16" s="49"/>
@@ -25180,9 +25180,9 @@
       <c r="Q16" s="38"/>
     </row>
     <row r="17" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A17" s="129"/>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
+      <c r="A17" s="130"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="132"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
       <c r="F17" s="50"/>
@@ -25218,13 +25218,13 @@
       <c r="Q18" s="58"/>
     </row>
     <row r="19" spans="1:17" ht="91.5" customHeight="1">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="130" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="130" t="s">
+      <c r="B19" s="131" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="131" t="s">
+      <c r="C19" s="132" t="s">
         <v>172</v>
       </c>
       <c r="D19" s="60" t="s">
@@ -25251,9 +25251,9 @@
       <c r="Q19" s="38"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="129"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
+      <c r="A20" s="130"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="132"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
       <c r="F20" s="49"/>
@@ -25270,9 +25270,9 @@
       <c r="Q20" s="38"/>
     </row>
     <row r="21" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A21" s="129"/>
-      <c r="B21" s="131"/>
-      <c r="C21" s="131"/>
+      <c r="A21" s="130"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="132"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
       <c r="F21" s="50"/>
@@ -25308,13 +25308,13 @@
       <c r="Q22" s="58"/>
     </row>
     <row r="23" spans="1:17" ht="51" customHeight="1">
-      <c r="A23" s="129" t="s">
+      <c r="A23" s="130" t="s">
         <v>159</v>
       </c>
-      <c r="B23" s="130" t="s">
+      <c r="B23" s="131" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="131" t="s">
+      <c r="C23" s="132" t="s">
         <v>166</v>
       </c>
       <c r="D23" s="60" t="s">
@@ -25341,9 +25341,9 @@
       <c r="Q23" s="38"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="129"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
+      <c r="A24" s="130"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="132"/>
       <c r="D24" s="48"/>
       <c r="E24" s="48"/>
       <c r="F24" s="49"/>
@@ -25360,9 +25360,9 @@
       <c r="Q24" s="38"/>
     </row>
     <row r="25" spans="1:17" ht="13.5" thickBot="1">
-      <c r="A25" s="129"/>
-      <c r="B25" s="131"/>
-      <c r="C25" s="131"/>
+      <c r="A25" s="130"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
       <c r="D25" s="48"/>
       <c r="E25" s="48"/>
       <c r="F25" s="50"/>
@@ -25399,25 +25399,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
@@ -25432,6 +25413,25 @@
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <conditionalFormatting sqref="F7:F9 G6:K6 M6:P9">
     <cfRule type="cellIs" priority="223" stopIfTrue="1" operator="equal">
@@ -25775,7 +25775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:II33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25818,25 +25818,25 @@
       </c>
       <c r="C1" s="65"/>
       <c r="D1" s="66"/>
-      <c r="E1" s="133" t="s">
+      <c r="E1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="144" t="s">
+      <c r="F1" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="150" t="s">
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="161"/>
+      <c r="K1" s="161"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="151"/>
-      <c r="Q1" s="152"/>
+      <c r="N1" s="148"/>
+      <c r="O1" s="148"/>
+      <c r="P1" s="148"/>
+      <c r="Q1" s="149"/>
       <c r="R1" s="38"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -26073,29 +26073,29 @@
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="69"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="153" t="s">
+      <c r="E2" s="150"/>
+      <c r="F2" s="136" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="145" t="s">
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="141" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="157" t="s">
+      <c r="N2" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="O2" s="157" t="s">
+      <c r="O2" s="133" t="s">
         <v>126</v>
       </c>
-      <c r="P2" s="157" t="s">
+      <c r="P2" s="133" t="s">
         <v>127</v>
       </c>
-      <c r="Q2" s="157" t="s">
+      <c r="Q2" s="133" t="s">
         <v>128</v>
       </c>
       <c r="R2" s="38"/>
@@ -26326,27 +26326,27 @@
       <c r="II2" s="1"/>
     </row>
     <row r="3" spans="1:243" s="6" customFormat="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="139" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="162" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="158"/>
-      <c r="O3" s="158"/>
-      <c r="P3" s="158"/>
-      <c r="Q3" s="158"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="134"/>
+      <c r="O3" s="134"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="134"/>
       <c r="R3" s="38"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -26575,23 +26575,23 @@
       <c r="II3" s="1"/>
     </row>
     <row r="4" spans="1:243" s="6" customFormat="1">
-      <c r="A4" s="161"/>
-      <c r="B4" s="135"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="155"/>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="J4" s="155"/>
-      <c r="K4" s="155"/>
-      <c r="L4" s="149"/>
-      <c r="M4" s="147"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
-      <c r="Q4" s="159"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="153"/>
+      <c r="D4" s="154"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="138"/>
+      <c r="K4" s="138"/>
+      <c r="L4" s="146"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="135"/>
+      <c r="Q4" s="135"/>
       <c r="R4" s="38"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -27320,13 +27320,13 @@
       <c r="II6" s="1"/>
     </row>
     <row r="7" spans="1:243" s="9" customFormat="1" ht="75">
-      <c r="A7" s="129">
+      <c r="A7" s="130">
         <v>1</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="131" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="132" t="s">
         <v>237</v>
       </c>
       <c r="D7" s="60" t="s">
@@ -27577,9 +27577,9 @@
       <c r="II7" s="13"/>
     </row>
     <row r="8" spans="1:243" s="9" customFormat="1" ht="57.75" customHeight="1">
-      <c r="A8" s="129"/>
-      <c r="B8" s="130"/>
-      <c r="C8" s="131"/>
+      <c r="A8" s="130"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="60" t="s">
         <v>134</v>
       </c>
@@ -27830,9 +27830,9 @@
       <c r="II8" s="13"/>
     </row>
     <row r="9" spans="1:243" s="9" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A9" s="129"/>
-      <c r="B9" s="130"/>
-      <c r="C9" s="131"/>
+      <c r="A9" s="130"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="132"/>
       <c r="D9" s="60"/>
       <c r="E9" s="75" t="s">
         <v>137</v>
@@ -28077,9 +28077,9 @@
       <c r="II9" s="13"/>
     </row>
     <row r="10" spans="1:243" s="9" customFormat="1" ht="38.25">
-      <c r="A10" s="129"/>
-      <c r="B10" s="131"/>
-      <c r="C10" s="131"/>
+      <c r="A10" s="130"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="132"/>
       <c r="D10" s="60"/>
       <c r="E10" s="60" t="s">
         <v>138</v>
@@ -28326,9 +28326,9 @@
       <c r="II10" s="13"/>
     </row>
     <row r="11" spans="1:243" s="9" customFormat="1" ht="77.25" thickBot="1">
-      <c r="A11" s="129"/>
-      <c r="B11" s="131"/>
-      <c r="C11" s="131"/>
+      <c r="A11" s="130"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
       <c r="D11" s="60"/>
       <c r="E11" s="75" t="s">
         <v>140</v>
@@ -28820,13 +28820,13 @@
       <c r="II12"/>
     </row>
     <row r="13" spans="1:243" s="9" customFormat="1" ht="75">
-      <c r="A13" s="129" t="s">
+      <c r="A13" s="130" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="130" t="s">
+      <c r="B13" s="131" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="131" t="s">
+      <c r="C13" s="132" t="s">
         <v>237</v>
       </c>
       <c r="D13" s="60" t="s">
@@ -29077,9 +29077,9 @@
       <c r="II13" s="13"/>
     </row>
     <row r="14" spans="1:243" s="9" customFormat="1" ht="51">
-      <c r="A14" s="129"/>
-      <c r="B14" s="130"/>
-      <c r="C14" s="131"/>
+      <c r="A14" s="130"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="60" t="s">
         <v>134</v>
       </c>
@@ -29330,9 +29330,9 @@
       <c r="II14" s="13"/>
     </row>
     <row r="15" spans="1:243" s="9" customFormat="1" ht="38.25">
-      <c r="A15" s="129"/>
-      <c r="B15" s="130"/>
-      <c r="C15" s="131"/>
+      <c r="A15" s="130"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="132"/>
       <c r="D15" s="60"/>
       <c r="E15" s="75" t="s">
         <v>137</v>
@@ -29577,9 +29577,9 @@
       <c r="II15" s="13"/>
     </row>
     <row r="16" spans="1:243" s="9" customFormat="1" ht="38.25">
-      <c r="A16" s="129"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
+      <c r="A16" s="130"/>
+      <c r="B16" s="132"/>
+      <c r="C16" s="132"/>
       <c r="D16" s="60"/>
       <c r="E16" s="60" t="s">
         <v>138</v>
@@ -29826,9 +29826,9 @@
       <c r="II16" s="13"/>
     </row>
     <row r="17" spans="1:243" s="9" customFormat="1" ht="39" thickBot="1">
-      <c r="A17" s="129"/>
-      <c r="B17" s="131"/>
-      <c r="C17" s="131"/>
+      <c r="A17" s="130"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="132"/>
       <c r="D17" s="60"/>
       <c r="E17" s="60" t="s">
         <v>144</v>
@@ -30320,13 +30320,13 @@
       <c r="II18"/>
     </row>
     <row r="19" spans="1:243" s="9" customFormat="1" ht="75">
-      <c r="A19" s="129">
+      <c r="A19" s="130">
         <v>3</v>
       </c>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="132" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="131" t="s">
+      <c r="C19" s="132" t="s">
         <v>130</v>
       </c>
       <c r="D19" s="60" t="s">
@@ -30577,9 +30577,9 @@
       <c r="II19" s="13"/>
     </row>
     <row r="20" spans="1:243" s="9" customFormat="1" ht="51">
-      <c r="A20" s="129"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="131"/>
+      <c r="A20" s="130"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="132"/>
       <c r="D20" s="60" t="s">
         <v>134</v>
       </c>
@@ -30830,9 +30830,9 @@
       <c r="II20" s="13"/>
     </row>
     <row r="21" spans="1:243" s="9" customFormat="1" ht="38.25">
-      <c r="A21" s="129"/>
-      <c r="B21" s="131"/>
-      <c r="C21" s="131"/>
+      <c r="A21" s="130"/>
+      <c r="B21" s="132"/>
+      <c r="C21" s="132"/>
       <c r="D21" s="48"/>
       <c r="E21" s="75" t="s">
         <v>137</v>
@@ -31077,9 +31077,9 @@
       <c r="II21" s="13"/>
     </row>
     <row r="22" spans="1:243" s="9" customFormat="1" ht="38.25">
-      <c r="A22" s="129"/>
-      <c r="B22" s="131"/>
-      <c r="C22" s="131"/>
+      <c r="A22" s="130"/>
+      <c r="B22" s="132"/>
+      <c r="C22" s="132"/>
       <c r="D22" s="48"/>
       <c r="E22" s="60" t="s">
         <v>138</v>
@@ -31326,9 +31326,9 @@
       <c r="II22" s="13"/>
     </row>
     <row r="23" spans="1:243" s="9" customFormat="1" ht="38.25">
-      <c r="A23" s="129"/>
-      <c r="B23" s="131"/>
-      <c r="C23" s="131"/>
+      <c r="A23" s="130"/>
+      <c r="B23" s="132"/>
+      <c r="C23" s="132"/>
       <c r="D23" s="48"/>
       <c r="E23" s="60" t="s">
         <v>144</v>
@@ -31573,9 +31573,9 @@
       <c r="II23" s="13"/>
     </row>
     <row r="24" spans="1:243" s="9" customFormat="1" ht="25.5">
-      <c r="A24" s="129"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="131"/>
+      <c r="A24" s="130"/>
+      <c r="B24" s="132"/>
+      <c r="C24" s="132"/>
       <c r="D24" s="48"/>
       <c r="E24" s="60" t="s">
         <v>147</v>
@@ -31820,9 +31820,9 @@
       <c r="II24" s="13"/>
     </row>
     <row r="25" spans="1:243" s="9" customFormat="1" ht="25.5">
-      <c r="A25" s="129"/>
-      <c r="B25" s="131"/>
-      <c r="C25" s="131"/>
+      <c r="A25" s="130"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="132"/>
       <c r="D25" s="48"/>
       <c r="E25" s="60" t="s">
         <v>148</v>
@@ -32067,9 +32067,9 @@
       <c r="II25" s="13"/>
     </row>
     <row r="26" spans="1:243" s="9" customFormat="1" ht="64.5" thickBot="1">
-      <c r="A26" s="129"/>
-      <c r="B26" s="131"/>
-      <c r="C26" s="131"/>
+      <c r="A26" s="130"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="132"/>
       <c r="D26" s="48"/>
       <c r="E26" s="60" t="s">
         <v>149</v>
@@ -34030,6 +34030,20 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="C19:C26"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="L1:L4"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="G2:G4"/>
@@ -34042,20 +34056,6 @@
     <mergeCell ref="O2:O4"/>
     <mergeCell ref="P2:P4"/>
     <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="L1:L4"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="B19:B26"/>
-    <mergeCell ref="C19:C26"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C13:C17"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K6 F7:F11 M6:Q6 M7:O7 Q7 M8:Q11">
     <cfRule type="cellIs" priority="123" stopIfTrue="1" operator="equal">
@@ -34410,11 +34410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -34440,152 +34440,152 @@
       <c r="A1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="170" t="s">
+      <c r="B1" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="171"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="173" t="s">
+      <c r="C1" s="187"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="186" t="s">
+      <c r="F1" s="194" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
-      <c r="I1" s="186"/>
-      <c r="J1" s="186"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="186"/>
-      <c r="M1" s="186"/>
-      <c r="N1" s="186"/>
-      <c r="O1" s="186"/>
-      <c r="P1" s="186"/>
-      <c r="Q1" s="186"/>
-      <c r="R1" s="186"/>
-      <c r="S1" s="187"/>
-      <c r="T1" s="189" t="s">
+      <c r="G1" s="194"/>
+      <c r="H1" s="194"/>
+      <c r="I1" s="194"/>
+      <c r="J1" s="194"/>
+      <c r="K1" s="194"/>
+      <c r="L1" s="194"/>
+      <c r="M1" s="194"/>
+      <c r="N1" s="194"/>
+      <c r="O1" s="194"/>
+      <c r="P1" s="194"/>
+      <c r="Q1" s="194"/>
+      <c r="R1" s="194"/>
+      <c r="S1" s="170"/>
+      <c r="T1" s="172" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="190"/>
-      <c r="V1" s="190"/>
-      <c r="W1" s="191"/>
+      <c r="U1" s="173"/>
+      <c r="V1" s="173"/>
+      <c r="W1" s="174"/>
       <c r="X1" s="89"/>
     </row>
     <row r="2" spans="1:24" ht="21.75" customHeight="1">
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="191" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="178" t="s">
+      <c r="C2" s="192"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="175" t="s">
         <v>261</v>
       </c>
-      <c r="G2" s="178" t="s">
+      <c r="G2" s="175" t="s">
         <v>262</v>
       </c>
-      <c r="H2" s="178" t="s">
+      <c r="H2" s="175" t="s">
         <v>263</v>
       </c>
-      <c r="I2" s="178" t="s">
+      <c r="I2" s="175" t="s">
         <v>264</v>
       </c>
-      <c r="J2" s="178" t="s">
+      <c r="J2" s="175" t="s">
         <v>230</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="175" t="s">
         <v>265</v>
       </c>
-      <c r="L2" s="178" t="s">
+      <c r="L2" s="175" t="s">
         <v>266</v>
       </c>
-      <c r="M2" s="178" t="s">
+      <c r="M2" s="175" t="s">
         <v>267</v>
       </c>
-      <c r="N2" s="178" t="s">
+      <c r="N2" s="175" t="s">
         <v>268</v>
       </c>
-      <c r="O2" s="178" t="s">
+      <c r="O2" s="175" t="s">
         <v>233</v>
       </c>
-      <c r="P2" s="178" t="s">
+      <c r="P2" s="175" t="s">
         <v>269</v>
       </c>
-      <c r="Q2" s="178" t="s">
+      <c r="Q2" s="175" t="s">
         <v>270</v>
       </c>
-      <c r="R2" s="178" t="s">
+      <c r="R2" s="175" t="s">
         <v>271</v>
       </c>
-      <c r="S2" s="187"/>
-      <c r="T2" s="192"/>
-      <c r="U2" s="192"/>
-      <c r="V2" s="192"/>
-      <c r="W2" s="192"/>
+      <c r="S2" s="170"/>
+      <c r="T2" s="178"/>
+      <c r="U2" s="178"/>
+      <c r="V2" s="178"/>
+      <c r="W2" s="178"/>
       <c r="X2" s="89"/>
     </row>
     <row r="3" spans="1:24" ht="21.75" customHeight="1">
       <c r="A3" s="87" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="175" t="s">
+      <c r="B3" s="191" t="s">
         <v>207</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="173"/>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
-      <c r="I3" s="179"/>
-      <c r="J3" s="179"/>
-      <c r="K3" s="179"/>
-      <c r="L3" s="179"/>
-      <c r="M3" s="179"/>
-      <c r="N3" s="179"/>
-      <c r="O3" s="179"/>
-      <c r="P3" s="179"/>
-      <c r="Q3" s="179"/>
-      <c r="R3" s="179"/>
-      <c r="S3" s="187"/>
-      <c r="T3" s="193"/>
-      <c r="U3" s="193"/>
-      <c r="V3" s="193"/>
-      <c r="W3" s="193"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="189"/>
+      <c r="F3" s="176"/>
+      <c r="G3" s="176"/>
+      <c r="H3" s="176"/>
+      <c r="I3" s="176"/>
+      <c r="J3" s="176"/>
+      <c r="K3" s="176"/>
+      <c r="L3" s="176"/>
+      <c r="M3" s="176"/>
+      <c r="N3" s="176"/>
+      <c r="O3" s="176"/>
+      <c r="P3" s="176"/>
+      <c r="Q3" s="176"/>
+      <c r="R3" s="176"/>
+      <c r="S3" s="170"/>
+      <c r="T3" s="179"/>
+      <c r="U3" s="179"/>
+      <c r="V3" s="179"/>
+      <c r="W3" s="179"/>
       <c r="X3" s="89"/>
     </row>
     <row r="4" spans="1:24" ht="26.25" customHeight="1">
       <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="175" t="s">
+      <c r="B4" s="191" t="s">
         <v>208</v>
       </c>
-      <c r="C4" s="176"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="174"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="180"/>
-      <c r="K4" s="180"/>
-      <c r="L4" s="180"/>
-      <c r="M4" s="180"/>
-      <c r="N4" s="180"/>
-      <c r="O4" s="180"/>
-      <c r="P4" s="180"/>
-      <c r="Q4" s="180"/>
-      <c r="R4" s="180"/>
-      <c r="S4" s="188"/>
-      <c r="T4" s="194"/>
-      <c r="U4" s="194"/>
-      <c r="V4" s="194"/>
-      <c r="W4" s="194"/>
+      <c r="C4" s="192"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="177"/>
+      <c r="J4" s="177"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="177"/>
+      <c r="M4" s="177"/>
+      <c r="N4" s="177"/>
+      <c r="O4" s="177"/>
+      <c r="P4" s="177"/>
+      <c r="Q4" s="177"/>
+      <c r="R4" s="177"/>
+      <c r="S4" s="171"/>
+      <c r="T4" s="180"/>
+      <c r="U4" s="180"/>
+      <c r="V4" s="180"/>
+      <c r="W4" s="180"/>
       <c r="X4" s="89"/>
     </row>
     <row r="5" spans="1:24">
@@ -34651,13 +34651,13 @@
       <c r="X6" s="89"/>
     </row>
     <row r="7" spans="1:24" ht="51">
-      <c r="A7" s="181" t="s">
+      <c r="A7" s="182" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="184" t="s">
+      <c r="B7" s="185" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="184" t="str">
+      <c r="C7" s="185" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -34692,9 +34692,9 @@
       <c r="X7" s="89"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="181"/>
-      <c r="B8" s="183"/>
-      <c r="C8" s="183"/>
+      <c r="A8" s="182"/>
+      <c r="B8" s="184"/>
+      <c r="C8" s="184"/>
       <c r="D8" s="97"/>
       <c r="E8" s="97"/>
       <c r="F8" s="101"/>
@@ -34718,9 +34718,9 @@
       <c r="X8" s="89"/>
     </row>
     <row r="9" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A9" s="181"/>
-      <c r="B9" s="183"/>
-      <c r="C9" s="183"/>
+      <c r="A9" s="182"/>
+      <c r="B9" s="184"/>
+      <c r="C9" s="184"/>
       <c r="D9" s="97"/>
       <c r="E9" s="97"/>
       <c r="F9" s="98"/>
@@ -34770,13 +34770,13 @@
       <c r="X10" s="107"/>
     </row>
     <row r="11" spans="1:24" ht="38.25">
-      <c r="A11" s="181" t="s">
+      <c r="A11" s="182" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="182" t="s">
+      <c r="B11" s="183" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="182" t="str">
+      <c r="C11" s="183" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -34821,9 +34821,9 @@
       <c r="X11" s="114"/>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="181"/>
-      <c r="B12" s="183"/>
-      <c r="C12" s="183"/>
+      <c r="A12" s="182"/>
+      <c r="B12" s="184"/>
+      <c r="C12" s="184"/>
       <c r="D12" s="97"/>
       <c r="E12" s="97"/>
       <c r="F12" s="101"/>
@@ -34847,9 +34847,9 @@
       <c r="X12" s="89"/>
     </row>
     <row r="13" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A13" s="181"/>
-      <c r="B13" s="183"/>
-      <c r="C13" s="183"/>
+      <c r="A13" s="182"/>
+      <c r="B13" s="184"/>
+      <c r="C13" s="184"/>
       <c r="D13" s="97"/>
       <c r="E13" s="97"/>
       <c r="F13" s="98"/>
@@ -34899,13 +34899,16 @@
       <c r="X14" s="107"/>
     </row>
     <row r="15" spans="1:24" ht="51">
-      <c r="A15" s="185" t="s">
+      <c r="A15" s="181" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="182" t="s">
+      <c r="B15" s="183" t="s">
         <v>214</v>
       </c>
-      <c r="C15" s="182"/>
+      <c r="C15" s="183" t="str">
+        <f>B3</f>
+        <v>Usuário Conectado ao sistema (Efetuado Login)</v>
+      </c>
       <c r="D15" s="108" t="str">
         <f>D11</f>
         <v>Sistema informará Conforme dados de entrada.</v>
@@ -34939,9 +34942,9 @@
       <c r="X15" s="114"/>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="181"/>
-      <c r="B16" s="183"/>
-      <c r="C16" s="183"/>
+      <c r="A16" s="182"/>
+      <c r="B16" s="184"/>
+      <c r="C16" s="184"/>
       <c r="D16" s="97"/>
       <c r="E16" s="97"/>
       <c r="F16" s="101"/>
@@ -34965,9 +34968,9 @@
       <c r="X16" s="89"/>
     </row>
     <row r="17" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A17" s="181"/>
-      <c r="B17" s="183"/>
-      <c r="C17" s="183"/>
+      <c r="A17" s="182"/>
+      <c r="B17" s="184"/>
+      <c r="C17" s="184"/>
       <c r="D17" s="97"/>
       <c r="E17" s="97"/>
       <c r="F17" s="98"/>
@@ -35017,13 +35020,13 @@
       <c r="X18" s="107"/>
     </row>
     <row r="19" spans="1:24" ht="102">
-      <c r="A19" s="185" t="s">
+      <c r="A19" s="181" t="s">
         <v>158</v>
       </c>
-      <c r="B19" s="182" t="s">
+      <c r="B19" s="183" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="182" t="str">
+      <c r="C19" s="183" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -35067,9 +35070,9 @@
       <c r="X19" s="114"/>
     </row>
     <row r="20" spans="1:24" ht="51">
-      <c r="A20" s="181"/>
-      <c r="B20" s="183"/>
-      <c r="C20" s="183"/>
+      <c r="A20" s="182"/>
+      <c r="B20" s="184"/>
+      <c r="C20" s="184"/>
       <c r="D20" s="97" t="s">
         <v>218</v>
       </c>
@@ -35099,9 +35102,9 @@
       <c r="X20" s="89"/>
     </row>
     <row r="21" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A21" s="181"/>
-      <c r="B21" s="183"/>
-      <c r="C21" s="183"/>
+      <c r="A21" s="182"/>
+      <c r="B21" s="184"/>
+      <c r="C21" s="184"/>
       <c r="D21" s="97"/>
       <c r="E21" s="97"/>
       <c r="F21" s="98"/>
@@ -35151,13 +35154,13 @@
       <c r="X22" s="107"/>
     </row>
     <row r="23" spans="1:24" ht="63.75">
-      <c r="A23" s="185" t="s">
+      <c r="A23" s="181" t="s">
         <v>159</v>
       </c>
-      <c r="B23" s="182" t="s">
+      <c r="B23" s="183" t="s">
         <v>287</v>
       </c>
-      <c r="C23" s="182" t="str">
+      <c r="C23" s="183" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -35202,9 +35205,9 @@
       <c r="X23" s="114"/>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="181"/>
-      <c r="B24" s="183"/>
-      <c r="C24" s="183"/>
+      <c r="A24" s="182"/>
+      <c r="B24" s="184"/>
+      <c r="C24" s="184"/>
       <c r="D24" s="97"/>
       <c r="E24" s="97"/>
       <c r="F24" s="101"/>
@@ -35228,9 +35231,9 @@
       <c r="X24" s="89"/>
     </row>
     <row r="25" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A25" s="181"/>
-      <c r="B25" s="183"/>
-      <c r="C25" s="183"/>
+      <c r="A25" s="182"/>
+      <c r="B25" s="184"/>
+      <c r="C25" s="184"/>
       <c r="D25" s="97"/>
       <c r="E25" s="97"/>
       <c r="F25" s="98"/>
@@ -35280,13 +35283,13 @@
       <c r="X26" s="107"/>
     </row>
     <row r="27" spans="1:24" ht="51">
-      <c r="A27" s="185" t="s">
+      <c r="A27" s="181" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="182" t="s">
+      <c r="B27" s="183" t="s">
         <v>222</v>
       </c>
-      <c r="C27" s="182" t="str">
+      <c r="C27" s="183" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -35327,9 +35330,9 @@
       <c r="X27" s="114"/>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="181"/>
-      <c r="B28" s="183"/>
-      <c r="C28" s="183"/>
+      <c r="A28" s="182"/>
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
       <c r="D28" s="97"/>
       <c r="E28" s="97"/>
       <c r="F28" s="101"/>
@@ -35353,9 +35356,9 @@
       <c r="X28" s="89"/>
     </row>
     <row r="29" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A29" s="181"/>
-      <c r="B29" s="183"/>
-      <c r="C29" s="183"/>
+      <c r="A29" s="182"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="184"/>
       <c r="D29" s="97"/>
       <c r="E29" s="97"/>
       <c r="F29" s="98"/>
@@ -35405,13 +35408,13 @@
       <c r="X30" s="107"/>
     </row>
     <row r="31" spans="1:24" ht="63.75">
-      <c r="A31" s="185" t="s">
+      <c r="A31" s="181" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="182" t="s">
+      <c r="B31" s="183" t="s">
         <v>224</v>
       </c>
-      <c r="C31" s="182" t="str">
+      <c r="C31" s="183" t="str">
         <f>B3</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -35451,9 +35454,9 @@
       <c r="X31" s="114"/>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="181"/>
-      <c r="B32" s="183"/>
-      <c r="C32" s="183"/>
+      <c r="A32" s="182"/>
+      <c r="B32" s="184"/>
+      <c r="C32" s="184"/>
       <c r="D32" s="97"/>
       <c r="E32" s="97"/>
       <c r="F32" s="101"/>
@@ -35477,9 +35480,9 @@
       <c r="X32" s="89"/>
     </row>
     <row r="33" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A33" s="181"/>
-      <c r="B33" s="183"/>
-      <c r="C33" s="183"/>
+      <c r="A33" s="182"/>
+      <c r="B33" s="184"/>
+      <c r="C33" s="184"/>
       <c r="D33" s="97"/>
       <c r="E33" s="97"/>
       <c r="F33" s="98"/>
@@ -35529,13 +35532,13 @@
       <c r="X34" s="107"/>
     </row>
     <row r="35" spans="1:24" ht="63.75">
-      <c r="A35" s="185" t="s">
+      <c r="A35" s="181" t="s">
         <v>162</v>
       </c>
-      <c r="B35" s="182" t="s">
+      <c r="B35" s="183" t="s">
         <v>226</v>
       </c>
-      <c r="C35" s="182" t="str">
+      <c r="C35" s="183" t="str">
         <f>C31</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -35572,9 +35575,9 @@
       <c r="X35" s="114"/>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" s="181"/>
-      <c r="B36" s="183"/>
-      <c r="C36" s="183"/>
+      <c r="A36" s="182"/>
+      <c r="B36" s="184"/>
+      <c r="C36" s="184"/>
       <c r="D36" s="97"/>
       <c r="E36" s="97"/>
       <c r="F36" s="101"/>
@@ -35598,9 +35601,9 @@
       <c r="X36" s="89"/>
     </row>
     <row r="37" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A37" s="181"/>
-      <c r="B37" s="183"/>
-      <c r="C37" s="183"/>
+      <c r="A37" s="182"/>
+      <c r="B37" s="184"/>
+      <c r="C37" s="184"/>
       <c r="D37" s="97"/>
       <c r="E37" s="97"/>
       <c r="F37" s="98"/>
@@ -35650,13 +35653,13 @@
       <c r="X38" s="107"/>
     </row>
     <row r="39" spans="1:24" ht="38.25">
-      <c r="A39" s="185" t="s">
+      <c r="A39" s="181" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="182" t="s">
+      <c r="B39" s="183" t="s">
         <v>228</v>
       </c>
-      <c r="C39" s="182" t="str">
+      <c r="C39" s="183" t="str">
         <f>C35</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -35690,9 +35693,9 @@
       <c r="X39" s="114"/>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" s="181"/>
-      <c r="B40" s="183"/>
-      <c r="C40" s="183"/>
+      <c r="A40" s="182"/>
+      <c r="B40" s="184"/>
+      <c r="C40" s="184"/>
       <c r="D40" s="97"/>
       <c r="E40" s="97"/>
       <c r="F40" s="101"/>
@@ -35716,9 +35719,9 @@
       <c r="X40" s="89"/>
     </row>
     <row r="41" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A41" s="181"/>
-      <c r="B41" s="183"/>
-      <c r="C41" s="183"/>
+      <c r="A41" s="182"/>
+      <c r="B41" s="184"/>
+      <c r="C41" s="184"/>
       <c r="D41" s="97"/>
       <c r="E41" s="97"/>
       <c r="F41" s="98"/>
@@ -35768,13 +35771,13 @@
       <c r="X42" s="107"/>
     </row>
     <row r="43" spans="1:24" ht="76.5">
-      <c r="A43" s="185" t="s">
+      <c r="A43" s="181" t="s">
         <v>234</v>
       </c>
-      <c r="B43" s="182" t="s">
+      <c r="B43" s="183" t="s">
         <v>292</v>
       </c>
-      <c r="C43" s="182" t="str">
+      <c r="C43" s="183" t="str">
         <f>C39</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -35817,9 +35820,9 @@
       <c r="X43" s="114"/>
     </row>
     <row r="44" spans="1:24">
-      <c r="A44" s="181"/>
-      <c r="B44" s="183"/>
-      <c r="C44" s="183"/>
+      <c r="A44" s="182"/>
+      <c r="B44" s="184"/>
+      <c r="C44" s="184"/>
       <c r="D44" s="97"/>
       <c r="E44" s="97"/>
       <c r="F44" s="101"/>
@@ -35843,9 +35846,9 @@
       <c r="X44" s="89"/>
     </row>
     <row r="45" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A45" s="181"/>
-      <c r="B45" s="183"/>
-      <c r="C45" s="183"/>
+      <c r="A45" s="182"/>
+      <c r="B45" s="184"/>
+      <c r="C45" s="184"/>
       <c r="D45" s="97"/>
       <c r="E45" s="97"/>
       <c r="F45" s="98"/>
@@ -35895,13 +35898,13 @@
       <c r="X46" s="107"/>
     </row>
     <row r="47" spans="1:24" ht="76.5">
-      <c r="A47" s="185" t="s">
+      <c r="A47" s="181" t="s">
         <v>165</v>
       </c>
-      <c r="B47" s="182" t="s">
+      <c r="B47" s="183" t="s">
         <v>231</v>
       </c>
-      <c r="C47" s="182" t="str">
+      <c r="C47" s="183" t="str">
         <f>C43</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -35944,9 +35947,9 @@
       <c r="X47" s="114"/>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="181"/>
-      <c r="B48" s="183"/>
-      <c r="C48" s="183"/>
+      <c r="A48" s="182"/>
+      <c r="B48" s="184"/>
+      <c r="C48" s="184"/>
       <c r="D48" s="97"/>
       <c r="E48" s="97"/>
       <c r="F48" s="101"/>
@@ -35970,9 +35973,9 @@
       <c r="X48" s="89"/>
     </row>
     <row r="49" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A49" s="181"/>
-      <c r="B49" s="183"/>
-      <c r="C49" s="183"/>
+      <c r="A49" s="182"/>
+      <c r="B49" s="184"/>
+      <c r="C49" s="184"/>
       <c r="D49" s="97"/>
       <c r="E49" s="97"/>
       <c r="F49" s="98"/>
@@ -36022,13 +36025,13 @@
       <c r="X50" s="107"/>
     </row>
     <row r="51" spans="1:24" ht="51">
-      <c r="A51" s="185" t="s">
+      <c r="A51" s="181" t="s">
         <v>235</v>
       </c>
-      <c r="B51" s="182" t="s">
+      <c r="B51" s="183" t="s">
         <v>295</v>
       </c>
-      <c r="C51" s="182" t="str">
+      <c r="C51" s="183" t="str">
         <f>C47</f>
         <v>Usuário Conectado ao sistema (Efetuado Login)</v>
       </c>
@@ -36066,9 +36069,9 @@
       <c r="X51" s="114"/>
     </row>
     <row r="52" spans="1:24">
-      <c r="A52" s="181"/>
-      <c r="B52" s="183"/>
-      <c r="C52" s="183"/>
+      <c r="A52" s="182"/>
+      <c r="B52" s="184"/>
+      <c r="C52" s="184"/>
       <c r="D52" s="97"/>
       <c r="E52" s="97"/>
       <c r="F52" s="101"/>
@@ -36092,9 +36095,9 @@
       <c r="X52" s="89"/>
     </row>
     <row r="53" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A53" s="181"/>
-      <c r="B53" s="183"/>
-      <c r="C53" s="183"/>
+      <c r="A53" s="182"/>
+      <c r="B53" s="184"/>
+      <c r="C53" s="184"/>
       <c r="D53" s="97"/>
       <c r="E53" s="97"/>
       <c r="F53" s="98"/>
@@ -36138,6 +36141,54 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F1:R1"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:C53"/>
     <mergeCell ref="S1:S4"/>
     <mergeCell ref="T1:W1"/>
     <mergeCell ref="L2:L4"/>
@@ -36151,54 +36202,6 @@
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
     <mergeCell ref="P2:P4"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F1:R1"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K6 M6:P9 M19:P21 M23:P25 F7:K9 M27:P29 F27:K29 M31:P33 F35:K37 M39:P41 F39:K41 M43:P45 F43:K45 M47:P49 M51:P53 F51:K53 F19:K21 F31:K33 M35:P37 F47:K49 F23:K25 F15:K17 M15:P17 F11:K13 M11:P13">
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>